<commit_message>
feat : creation of the six main windows
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\P_TodoList\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA69F05-D198-438F-8C3E-D50A57F62AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071963D5-983C-4A0C-954F-913B5097B6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="4320" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="objPlanifWeek" localSheetId="4">Planning!$A$1:$D$14</definedName>
     <definedName name="objPlanifWeek">PlanificationWeek!$A$1:$D$14</definedName>
     <definedName name="objRealizedWeek" localSheetId="5">achievementWeek!$A$1:$D$19</definedName>
-    <definedName name="objRealizedWeek" localSheetId="6">JNLTRAV!$A$1:$D$29</definedName>
+    <definedName name="objRealizedWeek" localSheetId="6">JNLTRAV!$A$1:$D$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Donnees!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
   <si>
     <t>Module :</t>
   </si>
@@ -226,19 +226,120 @@
 Recherches des normes et des éléments techniques à prendre en compte.</t>
   </si>
   <si>
-    <t>Création d'un git structuré et du fichier C#.
-Recherche outil pour la gestion de la méthode de projet : Clikup trouvé.</t>
-  </si>
-  <si>
     <t>Création du programme form, navigation entre les pages.</t>
-  </si>
-  <si>
-    <t>Fonctionnalités supplémentaires : gestion de la fenêtre d'affichage, etc.</t>
   </si>
   <si>
     <t>https://clickup.com/fr-FR/blog/113716/outils-de-gestion-de-projet-en-cascade
 https://app.clickup.com/
 https://www.freecodecamp.org/news/gitignore-file-how-to-ignore-files-and-folders-in-git/</t>
+  </si>
+  <si>
+    <t>Problème rencontré lors du premier commit. Problème résolu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chatgpt.com </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Création d'un git structuré et du fichier C#.
+Recherche outil pour la gestion de la méthode de projet : </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0066"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Clickup"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> trouvé.</t>
+    </r>
+  </si>
+  <si>
+    <t>Fonctionnalités supplémentaires.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Définitions des étapes de cette premières tâches sur le site web </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0066"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Clickup"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+Création des 6 pages de base. Début simplification du partage du nom de l'application (ralentissemment dû à un blocage). </t>
+    </r>
+  </si>
+  <si>
+    <t>Solution : revoir les projets passés.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lien de l'image :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://imjanehsieh.com/wp-content/uploads/2020/02/PDCA-8.png
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Logiciel pour conversion de l'image :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://convertio.co/fr/</t>
+    </r>
+  </si>
+  <si>
+    <t>&amp;&amp; 5 mn : Insertion d'un logo sur la page d'acceuil.  L'image a été converti au format .ico avant d'être insérée.</t>
   </si>
 </sst>
 </file>
@@ -248,7 +349,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -358,6 +459,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF0066"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -878,7 +993,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1155,6 +1270,10 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1166,6 +1285,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0066"/>
       <color rgb="FF28663D"/>
       <color rgb="FF1B952A"/>
       <color rgb="FF20B231"/>
@@ -2936,27 +3056,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2986,27 +3106,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3479,7 +3599,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3535,7 +3655,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="93" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="10"/>
     </row>
@@ -3662,7 +3782,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="92" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D17" s="9"/>
     </row>
@@ -4310,10 +4430,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4398,33 +4518,53 @@
         <v>4</v>
       </c>
       <c r="C6" s="93" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D6" s="94" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="94" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="53" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="94"/>
-    </row>
-    <row r="8" spans="1:4" s="53" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="94"/>
-    </row>
-    <row r="9" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="94"/>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="94" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -4477,319 +4617,595 @@
     <row r="18" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="94"/>
     </row>
     <row r="19" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="94"/>
     </row>
     <row r="20" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="94"/>
     </row>
     <row r="21" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="94"/>
     </row>
     <row r="22" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="94"/>
     </row>
     <row r="23" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
+      <c r="C23" s="93"/>
+      <c r="D23" s="94"/>
     </row>
     <row r="24" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="1"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="94"/>
     </row>
     <row r="25" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="51"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="94"/>
     </row>
     <row r="26" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-    </row>
-    <row r="27" spans="1:4" s="53" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="48">
-        <f>SUM(B3:B27)</f>
-        <v>13</v>
-      </c>
-      <c r="C28" s="90" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="49"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="50"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-    </row>
-    <row r="30" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="44">
-        <v>2</v>
-      </c>
-      <c r="C30" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="54">
-        <f>$D$1+7</f>
-        <v>45740</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="46" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="94"/>
+    </row>
+    <row r="27" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="94"/>
+    </row>
+    <row r="28" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="93"/>
+      <c r="D28" s="94"/>
+    </row>
+    <row r="29" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="93"/>
+      <c r="D29" s="94"/>
+    </row>
+    <row r="30" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="93"/>
+      <c r="D30" s="94"/>
+    </row>
+    <row r="31" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="94"/>
+    </row>
+    <row r="32" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="93"/>
+      <c r="D32" s="94"/>
+    </row>
+    <row r="33" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="93"/>
+      <c r="D33" s="94"/>
+    </row>
+    <row r="34" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-    </row>
-    <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="93"/>
+      <c r="D34" s="94"/>
+    </row>
+    <row r="35" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="20"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="20"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="20"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="20"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+    </row>
+    <row r="39" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="20"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+    </row>
+    <row r="40" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="38"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="20"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="20"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="20"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="20"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="51"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="20"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="51"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="20"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="20"/>
-    </row>
-    <row r="47" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="48" t="s">
+    </row>
+    <row r="42" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="51"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+    </row>
+    <row r="43" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="51"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+    </row>
+    <row r="44" spans="1:4" s="53" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="48">
-        <f>SUM(B32:B46)</f>
+      <c r="B45" s="48">
+        <f>SUM(B3:B44)</f>
+        <v>21</v>
+      </c>
+      <c r="C45" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="49"/>
+    </row>
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="50"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+    </row>
+    <row r="47" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="44">
+        <v>2</v>
+      </c>
+      <c r="C47" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="54">
+        <f>$D$1+7</f>
+        <v>45740</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="20"/>
+    </row>
+    <row r="81" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="32"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="34"/>
+      <c r="I81" s="20"/>
+    </row>
+    <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="31"/>
+      <c r="H82" s="31"/>
+      <c r="I82" s="20"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="38"/>
+      <c r="H83" s="38"/>
+      <c r="I83" s="20"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="20"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="38"/>
+      <c r="H85" s="38"/>
+      <c r="I85" s="20"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="37"/>
+      <c r="G86" s="38"/>
+      <c r="H86" s="38"/>
+      <c r="I86" s="20"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="38"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="20"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="20"/>
+      <c r="F88" s="37"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="20"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="37"/>
+      <c r="G89" s="38"/>
+      <c r="H89" s="38"/>
+      <c r="I89" s="20"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="51"/>
+      <c r="B90" s="51"/>
+      <c r="C90" s="52"/>
+      <c r="D90" s="52"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="20"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="51"/>
+      <c r="B91" s="51"/>
+      <c r="C91" s="52"/>
+      <c r="D91" s="52"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="39"/>
+      <c r="G91" s="40"/>
+      <c r="H91" s="40"/>
+      <c r="I91" s="20"/>
+    </row>
+    <row r="92" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="41"/>
+      <c r="G92" s="41"/>
+      <c r="H92" s="41"/>
+      <c r="I92" s="20"/>
+    </row>
+    <row r="93" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B93" s="48">
+        <f>SUM(B49:B92)</f>
         <v>0</v>
       </c>
-      <c r="C47" s="90" t="s">
+      <c r="C93" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D47" s="49"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-    </row>
-    <row r="48" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="91" t="s">
+      <c r="D93" s="49"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="20"/>
+      <c r="I93" s="20"/>
+    </row>
+    <row r="94" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A94" s="50"/>
+      <c r="B94" s="50"/>
+      <c r="C94" s="50"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
+      <c r="H94" s="20"/>
+      <c r="I94" s="20"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
+      <c r="H95" s="20"/>
+      <c r="I95" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="F45" xr:uid="{33845329-6629-4985-86D6-11E19AF8CA78}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="F91" xr:uid="{33845329-6629-4985-86D6-11E19AF8CA78}">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F37:F44 B3:B27 B32:B46" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F83:F90 B3:B44 B49:B92" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B28 B47" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B45 B93" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A27 A32:A46" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A44 A49:A92" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -4831,26 +5247,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5071,26 +5467,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5107,4 +5504,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : page layout of the current windows and redirections
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071963D5-983C-4A0C-954F-913B5097B6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A825C25-41C1-4E6C-A0C8-CB81A60DC83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4005" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
   <si>
     <t>Module :</t>
   </si>
@@ -340,6 +340,35 @@
   </si>
   <si>
     <t>&amp;&amp; 5 mn : Insertion d'un logo sur la page d'acceuil.  L'image a été converti au format .ico avant d'être insérée.</t>
+  </si>
+  <si>
+    <t>Partage du nom de l'application et de son logo entre toutes les pages.</t>
+  </si>
+  <si>
+    <t>Insertion des éléments graphiques propres à chaque fenêtre.
+Liaison des fenêtres entre elles grâce au clic sur bouton et la méthode show().
+Suite des recherches pour simplifier le partage du nom de l'application (et de son logo).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Erreur rencontrée lors de la compilation du fichier. Solution </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: https://webdevdesigner.com/q/visual-studio-build-fails-unable-to-copy-exe-file-from-obj-debug-to-bin-debug-68675/</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1260,20 +1289,20 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1993,7 +2022,7 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -2211,10 +2240,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="96"/>
+      <c r="C19" s="97"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -3165,7 +3194,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3174,7 +3203,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="98"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3598,8 +3627,8 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4432,8 +4461,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4548,7 +4577,7 @@
       <c r="C8" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="99" t="s">
+      <c r="D8" s="95" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4566,21 +4595,39 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="93"/>
+    <row r="10" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="C10" s="93" t="s">
+        <v>61</v>
+      </c>
       <c r="D10" s="94"/>
     </row>
-    <row r="11" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="94"/>
-    </row>
-    <row r="12" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+    <row r="11" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="93" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="53" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
       <c r="C12" s="93"/>
       <c r="D12" s="94"/>
     </row>
@@ -4782,7 +4829,7 @@
       </c>
       <c r="B45" s="48">
         <f>SUM(B3:B44)</f>
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C45" s="90" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
feat : initialization of the database and its content
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A825C25-41C1-4E6C-A0C8-CB81A60DC83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2679A61D-94DD-441D-B844-9BA77D52DB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4005" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
   <si>
     <t>Module :</t>
   </si>
@@ -269,6 +269,80 @@
     <t>Fonctionnalités supplémentaires.</t>
   </si>
   <si>
+    <t>Partage du nom de l'application et de son logo entre toutes les pages.</t>
+  </si>
+  <si>
+    <t>Insertion des éléments graphiques propres à chaque fenêtre.
+Liaison des fenêtres entre elles grâce au clic sur bouton et la méthode show().
+Suite des recherches pour simplifier le partage du nom de l'application (et de son logo).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Erreur rencontrée lors de la compilation du fichier. Solution </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: https://webdevdesigner.com/q/visual-studio-build-fails-unable-to-copy-exe-file-from-obj-debug-to-bin-debug-68675/</t>
+    </r>
+  </si>
+  <si>
+    <t>Création des modèles MCD, MLDP.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Recherche d'une solution  pour simplifier le modèle MCD qui a 5 types d'association entre seulement 2 entités, mais : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://bliaudet.free.fr/IMG/pdf/Modelisation-03-MEA-1-Cours-TD.pdf</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Source d'info pour le second script :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://www.ibm.com/docs/fr/rpt/9.5?topic=datasets-creating-dataset-associated-test</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Définitions des étapes de cette premières tâches sur le site web </t>
     </r>
@@ -290,33 +364,25 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">.
-Création des 6 pages de base. Début simplification du partage du nom de l'application (ralentissemment dû à un blocage). </t>
+      <t>.
+Création des 6 pages de base. Début simplification du partage du nom de l'application (ralentissemment dû à un blocage). 
+Insertion d'un logo sur la page d'acceuil.  L'image a été converti au format .ico avant d'être insérée.</t>
     </r>
   </si>
   <si>
-    <t>Solution : revoir les projets passés.</t>
-  </si>
-  <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Lien de l'image :</t>
+      <t xml:space="preserve">Piste pour m'aider : revoir les projets passés.
+Lien de l'image : </t>
     </r>
     <r>
       <rPr>
         <u/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> https://imjanehsieh.com/wp-content/uploads/2020/02/PDCA-8.png
-</t>
+      <t>https://imjanehsieh.com/wp-content/uploads/2020/02/PDCA-8.png</t>
     </r>
     <r>
       <rPr>
@@ -325,50 +391,30 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Logiciel pour conversion de l'image :</t>
+      <t xml:space="preserve">
+Logiciel pour conversion de l'image : </t>
     </r>
     <r>
       <rPr>
         <u/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> https://convertio.co/fr/</t>
+      <t>https://convertio.co/fr/</t>
     </r>
   </si>
   <si>
-    <t>&amp;&amp; 5 mn : Insertion d'un logo sur la page d'acceuil.  L'image a été converti au format .ico avant d'être insérée.</t>
-  </si>
-  <si>
-    <t>Partage du nom de l'application et de son logo entre toutes les pages.</t>
-  </si>
-  <si>
-    <t>Insertion des éléments graphiques propres à chaque fenêtre.
-Liaison des fenêtres entre elles grâce au clic sur bouton et la méthode show().
-Suite des recherches pour simplifier le partage du nom de l'application (et de son logo).</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Erreur rencontrée lors de la compilation du fichier. Solution </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>: https://webdevdesigner.com/q/visual-studio-build-fails-unable-to-copy-exe-file-from-obj-debug-to-bin-debug-68675/</t>
-    </r>
+    <t xml:space="preserve">Création du script MPD.
+Recherche concernant le deuxième script à produire (script laissé pour la fin).
+Logiciel uWAMP délaissé pour Docker après recherches d'installation portable.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialisation du conteneur "Docker".
+Script d'initialisation de la base de données. Importation réussie.
+</t>
   </si>
 </sst>
 </file>
@@ -378,7 +424,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -499,6 +545,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -3627,7 +3680,7 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -4461,8 +4514,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4567,80 +4620,92 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="53" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="93" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C9" s="93" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="94" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D9" s="94"/>
+    </row>
+    <row r="10" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="93" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="94"/>
-    </row>
-    <row r="11" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D10" s="94" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="53" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C11" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="94" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="53" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" s="53" customFormat="1" ht="54" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
       </c>
-      <c r="C12" s="93"/>
-      <c r="D12" s="94"/>
-    </row>
-    <row r="13" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="93"/>
+      <c r="C12" s="93" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="94" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
+      <c r="C13" s="93" t="s">
+        <v>65</v>
+      </c>
       <c r="D13" s="94"/>
     </row>
     <row r="14" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="93"/>
+      <c r="C14" s="93">
+        <v>10</v>
+      </c>
       <c r="D14" s="94"/>
     </row>
     <row r="15" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
@@ -4829,7 +4894,7 @@
       </c>
       <c r="B45" s="48">
         <f>SUM(B3:B44)</f>
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C45" s="90" t="s">
         <v>37</v>
@@ -5245,14 +5310,14 @@
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F83:F90 B3:B44 B49:B92" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F83:F90 B49:B92 B3:B44" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B45 B93" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A44 A49:A92" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A49:A92 A3:A44" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
feat : MVC model and creation of the page database.cs to link the APP with the DB
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2679A61D-94DD-441D-B844-9BA77D52DB28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563A4E44-7C4C-469E-A0DD-56D101ACB7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="74">
   <si>
     <t>Module :</t>
   </si>
@@ -340,33 +340,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> https://www.ibm.com/docs/fr/rpt/9.5?topic=datasets-creating-dataset-associated-test</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Définitions des étapes de cette premières tâches sur le site web </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0066"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Clickup"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.
-Création des 6 pages de base. Début simplification du partage du nom de l'application (ralentissemment dû à un blocage). 
-Insertion d'un logo sur la page d'acceuil.  L'image a été converti au format .ico avant d'être insérée.</t>
     </r>
   </si>
   <si>
@@ -416,6 +389,142 @@
 Script d'initialisation de la base de données. Importation réussie.
 </t>
   </si>
+  <si>
+    <t>Absence.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Définitions des étapes de cette première tâche sur le site web </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FFFF0066"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Clickup"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+Création des 6 pages de base. Début simplification du partage du nom de l'application (ralentissemment dû à un blocage). 
+Insertion d'un logo sur la page d'acceuil.  L'image a été converti au format .ico avant d'être insérée.</t>
+    </r>
+  </si>
+  <si>
+    <t>Mise en place du modèle MVC de base.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Lien d'aide pour les requêtes MySQL depuis C# : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://stackoverflow.com/questions/21618015/how-to-connect-to-mysql-database</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Lien d'installation du paquet :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://www.nuget.org/packages/MySql.Data/</t>
+    </r>
+  </si>
+  <si>
+    <t>Introduction du cours avec M. Benfares.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implémentation d'un "Try -Catch".
+Installation du paquet MySQL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF1B952A"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>grâce à l'aide d'un camarade</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C# Exceptions (Try..Catch) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lien d'aide pour l'installation du paquet :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://ourcodeworld.com/articles/read/218/how-to-connect-to-mysql-with-c-sharp-winforms-and-xampp</t>
+    </r>
+  </si>
+  <si>
+    <t>Création de la page "database.cs" pour les requêtes. Code pour se connecter à la DB créé. 
+Difficultés à utiliser la directive MySQL pour lier la base de données à l'application - installation d'un paquet, pour m'aider, infructueux.</t>
+  </si>
+  <si>
+    <t>Retard dû à un problème d'ouverture de session sur le desktop.
+Requêtes de base depuis l'application.</t>
+  </si>
 </sst>
 </file>
 
@@ -424,7 +533,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -555,6 +664,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF1B952A"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1075,7 +1192,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1356,6 +1473,13 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1367,9 +1491,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF1B952A"/>
       <color rgb="FFFF0066"/>
       <color rgb="FF28663D"/>
-      <color rgb="FF1B952A"/>
       <color rgb="FF20B231"/>
     </mruColors>
   </colors>
@@ -3138,27 +3262,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3188,27 +3312,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3680,8 +3804,8 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4514,8 +4638,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4628,10 +4752,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="93" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="95" t="s">
         <v>62</v>
-      </c>
-      <c r="D8" s="95" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
@@ -4682,7 +4806,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="93" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="94" t="s">
         <v>61</v>
@@ -4696,46 +4820,84 @@
         <v>4</v>
       </c>
       <c r="C13" s="93" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="94"/>
+    </row>
+    <row r="14" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2">
+        <v>12</v>
+      </c>
+      <c r="C14" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="94"/>
-    </row>
-    <row r="14" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="93">
-        <v>10</v>
-      </c>
       <c r="D14" s="94"/>
     </row>
     <row r="15" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="93"/>
+      <c r="A15" s="100" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="93" t="s">
+        <v>69</v>
+      </c>
       <c r="D15" s="94"/>
     </row>
-    <row r="16" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="93"/>
+    <row r="16" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+      <c r="C16" s="93" t="s">
+        <v>67</v>
+      </c>
       <c r="D16" s="94"/>
     </row>
-    <row r="17" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="94"/>
-    </row>
-    <row r="18" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="94"/>
-    </row>
-    <row r="19" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="93"/>
+    <row r="17" spans="1:4" s="53" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+      <c r="C17" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="94" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="53" customFormat="1" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2">
+        <v>4</v>
+      </c>
+      <c r="C18" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="101" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4</v>
+      </c>
+      <c r="C19" s="93" t="s">
+        <v>73</v>
+      </c>
       <c r="D19" s="94"/>
     </row>
     <row r="20" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
@@ -4894,7 +5056,7 @@
       </c>
       <c r="B45" s="48">
         <f>SUM(B3:B44)</f>
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="C45" s="90" t="s">
         <v>37</v>
@@ -5323,16 +5485,18 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" display="https://clickup.com/fr-FR/blog/113716/outils-de-gestion-de-projet-en-cascade" xr:uid="{DA8F090E-F7C9-447F-A025-675A43AE436C}"/>
+    <hyperlink ref="D17" r:id="rId2" display="https://www.nuget.org/packages/MySql.Data/" xr:uid="{D2F02347-FCC7-43CE-AD4D-A5D7157C9DB5}"/>
+    <hyperlink ref="D18" r:id="rId3" display="https://www.w3schools.com/cs/cs_exceptions.php" xr:uid="{FA400CED-9B11-481C-8A43-4789B8DC1C63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId5" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+        <control shapeId="43009" r:id="rId7" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5351,7 +5515,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId5" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId7" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5359,6 +5523,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5579,27 +5763,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5616,23 +5799,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : Fusion of the Database.cs file with the Model.cs. Code to validate the connexion of an user and start of code to manage tasks.
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563A4E44-7C4C-469E-A0DD-56D101ACB7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB10110B-64AF-4BF8-9E3A-DD2B4BF6AC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
   <si>
     <t>Module :</t>
   </si>
@@ -418,9 +418,6 @@
 Création des 6 pages de base. Début simplification du partage du nom de l'application (ralentissemment dû à un blocage). 
 Insertion d'un logo sur la page d'acceuil.  L'image a été converti au format .ico avant d'être insérée.</t>
     </r>
-  </si>
-  <si>
-    <t>Mise en place du modèle MVC de base.</t>
   </si>
   <si>
     <r>
@@ -522,8 +519,64 @@
 Difficultés à utiliser la directive MySQL pour lier la base de données à l'application - installation d'un paquet, pour m'aider, infructueux.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lien pour créer des noms aléatoires :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://fullnamegenerator.com/fr/</t>
+    </r>
+  </si>
+  <si>
+    <t>Requêtes de base implémentées (vérification de la connexion, ajout, modification et suppression des tâches) dans l'application et tester dans phpMyAdmin.</t>
+  </si>
+  <si>
     <t>Retard dû à un problème d'ouverture de session sur le desktop.
-Requêtes de base depuis l'application.</t>
+Début implémentation des requêtes de base.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Pour savoir comment exécuter des requêtes MySQL en C# : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://www.delftstack.com/fr/howto/csharp/csharp-sql-select/</t>
+    </r>
+  </si>
+  <si>
+    <t>Mise en place du modèle MVC de base (erreurs secondaires laissées de côté).</t>
+  </si>
+  <si>
+    <t>Correction des erreurs dans le code dû à certaines données pas en adéquation avec le modèle MVC.</t>
+  </si>
+  <si>
+    <t>Code pour le test de la connexion implémenté.
+Fusion du fichier "Database.cs" avec "Model.cs" pour éviter des redondances de fonctions et ne garder que "Model.cs".
+Début de code pour faire des CRUD sur une tâche.</t>
   </si>
 </sst>
 </file>
@@ -1463,16 +1516,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1480,6 +1523,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2417,10 +2470,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="97"/>
+      <c r="C19" s="99"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -3251,7 +3304,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ETML L,Normal"ETML&amp;C&amp;"-,Normal"Planification&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"-,Normal"&amp;D - GGZ&amp;C&amp;"-,Normal"&amp;F - &amp;A&amp;R&amp;"-,Normal"Page &amp;P/&amp;N</oddFooter>
@@ -3262,27 +3315,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3312,27 +3365,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3371,7 +3424,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="100" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3380,7 +3433,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="99"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3804,7 +3857,7 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -4638,8 +4691,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4822,7 +4875,9 @@
       <c r="C13" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="94"/>
+      <c r="D13" s="94" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -4837,14 +4892,14 @@
       <c r="D14" s="94"/>
     </row>
     <row r="15" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="100" t="s">
+      <c r="A15" s="96" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
       </c>
       <c r="C15" s="93" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="94"/>
     </row>
@@ -4856,7 +4911,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="93" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D16" s="94"/>
     </row>
@@ -4868,10 +4923,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="93" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="94" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="53" customFormat="1" ht="64.5" x14ac:dyDescent="0.25">
@@ -4882,10 +4937,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="97" t="s">
         <v>70</v>
-      </c>
-      <c r="D18" s="101" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
@@ -4896,26 +4951,46 @@
         <v>4</v>
       </c>
       <c r="C19" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="94"/>
+    </row>
+    <row r="20" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4</v>
+      </c>
+      <c r="C20" s="93" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="94"/>
-    </row>
-    <row r="20" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="94"/>
-    </row>
-    <row r="21" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="93"/>
+      <c r="D20" s="94" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="53" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
+      <c r="C21" s="93" t="s">
+        <v>77</v>
+      </c>
       <c r="D21" s="94"/>
     </row>
-    <row r="22" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="93"/>
+    <row r="22" spans="1:4" s="53" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4</v>
+      </c>
+      <c r="C22" s="93" t="s">
+        <v>78</v>
+      </c>
       <c r="D22" s="94"/>
     </row>
     <row r="23" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
@@ -5056,7 +5131,7 @@
       </c>
       <c r="B45" s="48">
         <f>SUM(B3:B44)</f>
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C45" s="90" t="s">
         <v>37</v>
@@ -5523,26 +5598,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5763,26 +5818,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5799,4 +5855,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs : creation of a file for the encountered error in the app
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB10110B-64AF-4BF8-9E3A-DD2B4BF6AC12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6242E54-D5F1-4D5C-B3D6-641B23933957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="objPlanifWeek" localSheetId="4">Planning!$A$1:$D$14</definedName>
     <definedName name="objPlanifWeek">PlanificationWeek!$A$1:$D$14</definedName>
     <definedName name="objRealizedWeek" localSheetId="5">achievementWeek!$A$1:$D$19</definedName>
-    <definedName name="objRealizedWeek" localSheetId="6">JNLTRAV!$A$1:$D$46</definedName>
+    <definedName name="objRealizedWeek" localSheetId="6">JNLTRAV!$A$1:$D$24</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Donnees!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="82">
   <si>
     <t>Module :</t>
   </si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t>Toutes les tâches supplémentaires qui se seraient ajoutées.</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
   <si>
     <t>Documentation complète du projet.
@@ -571,12 +568,28 @@
     <t>Mise en place du modèle MVC de base (erreurs secondaires laissées de côté).</t>
   </si>
   <si>
-    <t>Correction des erreurs dans le code dû à certaines données pas en adéquation avec le modèle MVC.</t>
-  </si>
-  <si>
-    <t>Code pour le test de la connexion implémenté.
+    <t>Correction des erreurs dans le code dû à certaines données pas en adéquation avec le modèle MVC.
+Code pour le test de la connexion implémenté.
 Fusion du fichier "Database.cs" avec "Model.cs" pour éviter des redondances de fonctions et ne garder que "Model.cs".
 Début de code pour faire des CRUD sur une tâche.</t>
+  </si>
+  <si>
+    <t>(en prévision.)</t>
+  </si>
+  <si>
+    <t>Recherche de solutions pour résoudre mon problème (voir erreur n° 6 du rapport).</t>
+  </si>
+  <si>
+    <t>Résolution de l'erreur. 
+Nouvelle erreur empêchant l'ouverture de "TasksTodoPage".
+Création du fichier .log pour les erreurs.</t>
+  </si>
+  <si>
+    <t>Difficulté à résoudre l'erreur actuelle (n° 7).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demande d'aide de mon chef de prof (M. Schaffter) et d'un camarade. 
+Utilisation de chatGPT également infructueuse. </t>
   </si>
 </sst>
 </file>
@@ -3304,7 +3317,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ETML L,Normal"ETML&amp;C&amp;"-,Normal"Planification&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"-,Normal"&amp;D - GGZ&amp;C&amp;"-,Normal"&amp;F - &amp;A&amp;R&amp;"-,Normal"Page &amp;P/&amp;N</oddFooter>
@@ -3315,27 +3328,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3365,27 +3378,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3858,7 +3871,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3902,7 +3915,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="9"/>
     </row>
@@ -3914,7 +3927,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="93" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="10"/>
     </row>
@@ -3962,7 +3975,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="93" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="D8" s="10"/>
     </row>
@@ -4041,7 +4054,7 @@
         <v>20</v>
       </c>
       <c r="C17" s="92" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="9"/>
     </row>
@@ -4053,7 +4066,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="93" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="10"/>
     </row>
@@ -4099,7 +4112,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="93" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="20"/>
@@ -4689,10 +4702,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4741,7 +4754,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="92" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="9"/>
     </row>
@@ -4753,7 +4766,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="93" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="10"/>
     </row>
@@ -4765,7 +4778,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="93" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="10"/>
     </row>
@@ -4777,10 +4790,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="94" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
@@ -4791,10 +4804,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="93" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="94" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" s="94" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="53" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
@@ -4805,10 +4818,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="93" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="95" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
@@ -4819,7 +4832,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="93" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="94"/>
     </row>
@@ -4831,10 +4844,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="93" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="94" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="53" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
@@ -4845,10 +4858,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="94" t="s">
         <v>59</v>
-      </c>
-      <c r="D11" s="94" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="53" customFormat="1" ht="54" x14ac:dyDescent="0.25">
@@ -4859,10 +4872,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="93" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="94" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
@@ -4873,10 +4886,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="94" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
@@ -4887,7 +4900,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="93" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="94"/>
     </row>
@@ -4899,7 +4912,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="93" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="94"/>
     </row>
@@ -4911,7 +4924,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="93" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="94"/>
     </row>
@@ -4923,10 +4936,10 @@
         <v>4</v>
       </c>
       <c r="C17" s="93" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D17" s="94" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="53" customFormat="1" ht="64.5" x14ac:dyDescent="0.25">
@@ -4937,10 +4950,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="93" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="97" t="s">
         <v>69</v>
-      </c>
-      <c r="D18" s="97" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
@@ -4951,7 +4964,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="94"/>
     </row>
@@ -4963,13 +4976,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="93" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="94" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="53" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="53" customFormat="1" ht="81" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -4977,584 +4990,351 @@
         <v>4</v>
       </c>
       <c r="C21" s="93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="94"/>
     </row>
-    <row r="22" spans="1:4" s="53" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="53" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>27</v>
+      </c>
+      <c r="C22" s="93" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="94"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="48">
+        <f>SUM(B3:B22)</f>
+        <v>111</v>
+      </c>
+      <c r="C23" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="49"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="50"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="44">
+        <v>2</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="54">
+        <f>$D$1+7</f>
+        <v>45740</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B27" s="4">
         <v>4</v>
       </c>
-      <c r="C22" s="93" t="s">
+      <c r="C27" s="92" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="94"/>
-    </row>
-    <row r="23" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="94"/>
-    </row>
-    <row r="24" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="94"/>
-    </row>
-    <row r="25" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="93"/>
-      <c r="D25" s="94"/>
-    </row>
-    <row r="26" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="94"/>
-    </row>
-    <row r="27" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="93"/>
-      <c r="D27" s="94"/>
-    </row>
-    <row r="28" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="93"/>
-      <c r="D28" s="94"/>
-    </row>
-    <row r="29" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="94"/>
-    </row>
-    <row r="30" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="94"/>
-    </row>
-    <row r="31" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4</v>
+      </c>
+      <c r="C28" s="93" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A30" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2</v>
+      </c>
+      <c r="C30" s="93" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="94"/>
-    </row>
-    <row r="32" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="93"/>
-      <c r="D32" s="94"/>
-    </row>
-    <row r="33" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="94"/>
-    </row>
-    <row r="34" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="93"/>
-      <c r="D34" s="94"/>
-    </row>
-    <row r="35" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="51"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-    </row>
-    <row r="43" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="51"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
-    </row>
-    <row r="44" spans="1:4" s="53" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="48">
-        <f>SUM(B3:B44)</f>
-        <v>88</v>
-      </c>
-      <c r="C45" s="90" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="49"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="50"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-    </row>
-    <row r="47" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" s="44">
-        <v>2</v>
-      </c>
-      <c r="C47" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="54">
-        <f>$D$1+7</f>
-        <v>45740</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="46" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+    </row>
+    <row r="59" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="10"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="10"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="20"/>
-      <c r="H80" s="20"/>
-      <c r="I80" s="20"/>
-    </row>
-    <row r="81" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="33"/>
-      <c r="H81" s="34"/>
-      <c r="I81" s="20"/>
-    </row>
-    <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="10"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="31"/>
-      <c r="H82" s="31"/>
-      <c r="I82" s="20"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="10"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="38"/>
-      <c r="H83" s="38"/>
-      <c r="I83" s="20"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="38"/>
-      <c r="H84" s="38"/>
-      <c r="I84" s="20"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="10"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="37"/>
-      <c r="G85" s="38"/>
-      <c r="H85" s="38"/>
-      <c r="I85" s="20"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="37"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="38"/>
-      <c r="I86" s="20"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="38"/>
-      <c r="I87" s="20"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="20"/>
-      <c r="F88" s="37"/>
-      <c r="G88" s="38"/>
-      <c r="H88" s="38"/>
-      <c r="I88" s="20"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="37"/>
-      <c r="G89" s="38"/>
-      <c r="H89" s="38"/>
-      <c r="I89" s="20"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="51"/>
-      <c r="B90" s="51"/>
-      <c r="C90" s="52"/>
-      <c r="D90" s="52"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="37"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="38"/>
-      <c r="I90" s="20"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="51"/>
-      <c r="B91" s="51"/>
-      <c r="C91" s="52"/>
-      <c r="D91" s="52"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="39"/>
-      <c r="G91" s="40"/>
-      <c r="H91" s="40"/>
-      <c r="I91" s="20"/>
-    </row>
-    <row r="92" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="41"/>
-      <c r="G92" s="41"/>
-      <c r="H92" s="41"/>
-      <c r="I92" s="20"/>
-    </row>
-    <row r="93" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="48" t="s">
+      <c r="E59" s="20"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="33"/>
+      <c r="H59" s="34"/>
+      <c r="I59" s="20"/>
+    </row>
+    <row r="60" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B93" s="48">
-        <f>SUM(B49:B92)</f>
-        <v>0</v>
-      </c>
-      <c r="C93" s="90" t="s">
+      <c r="B60" s="48">
+        <f>SUM(B27:B59)</f>
+        <v>14</v>
+      </c>
+      <c r="C60" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D93" s="49"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="20"/>
-      <c r="G93" s="20"/>
-      <c r="H93" s="20"/>
-      <c r="I93" s="20"/>
-    </row>
-    <row r="94" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A94" s="50"/>
-      <c r="B94" s="50"/>
-      <c r="C94" s="50"/>
-      <c r="D94" s="50"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="20"/>
-      <c r="H94" s="20"/>
-      <c r="I94" s="20"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="91" t="s">
+      <c r="D60" s="49"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+    </row>
+    <row r="61" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A61" s="50"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="20"/>
-      <c r="H95" s="20"/>
-      <c r="I95" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="F91" xr:uid="{33845329-6629-4985-86D6-11E19AF8CA78}">
-      <formula1>0</formula1>
-      <formula2>DureePeriode-1</formula2>
-    </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="F83:F90 B49:B92 B3:B44" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+  <dataValidations count="3">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B27:B59 B3:B22" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B45 B93" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B60" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A49:A92 A3:A44" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27:A59 A3:A22" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -5598,6 +5378,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5818,27 +5618,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5855,23 +5654,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : access to the app by a known user, start of adding and displaying of an user tasks
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6242E54-D5F1-4D5C-B3D6-641B23933957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D9A150-87D1-4ADC-A4E5-8BE84B7FC519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5985" yWindow="3900" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
   <si>
     <t>Module :</t>
   </si>
@@ -568,12 +568,6 @@
     <t>Mise en place du modèle MVC de base (erreurs secondaires laissées de côté).</t>
   </si>
   <si>
-    <t>Correction des erreurs dans le code dû à certaines données pas en adéquation avec le modèle MVC.
-Code pour le test de la connexion implémenté.
-Fusion du fichier "Database.cs" avec "Model.cs" pour éviter des redondances de fonctions et ne garder que "Model.cs".
-Début de code pour faire des CRUD sur une tâche.</t>
-  </si>
-  <si>
     <t>(en prévision.)</t>
   </si>
   <si>
@@ -588,8 +582,26 @@
     <t>Difficulté à résoudre l'erreur actuelle (n° 7).</t>
   </si>
   <si>
-    <t xml:space="preserve">Demande d'aide de mon chef de prof (M. Schaffter) et d'un camarade. 
-Utilisation de chatGPT également infructueuse. </t>
+    <t>Demande d'aide à mon chef de prof (M. Schaffter) et à un camarade. 
+Utilisation de chatGPT partiellement utile (enlever string.Format()); l'aide de mon camarade a permis la résolution complète de l'erreur (séparation du nom du serveur du n° de port).</t>
+  </si>
+  <si>
+    <t>Correction des erreurs dans le code dû à certaines données pas en adéquation avec le modèle MVC.
+Code pour le test de la connexion utilisateur implémenté.
+Fusion du fichier "Database.cs" avec "Model.cs" pour éviter des redondances de fonctions et ne garder que "Model.cs".
+Début de code pour faire des CRUD sur une tâche.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changement des redirections pour correspondre au modèle MVC.
+Implémentation d'une gestion d'erreur en cas d'authentifiaction non reconnue. </t>
+  </si>
+  <si>
+    <t>https://prog101.com/exemples/csharp/chaines/compter-nombre-mot-dans-chaine.php</t>
+  </si>
+  <si>
+    <t>Recherche d'un moyen de compter le nombre de mot dans la tâche avant validation et ajout à la liste des tâches.
+Ajout de la tâche au tableau à vérifie.
+Affichage des tâches contenues dans la DB en cours.</t>
   </si>
 </sst>
 </file>
@@ -3328,27 +3340,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3378,27 +3390,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3870,7 +3882,7 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -3975,7 +3987,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="10"/>
     </row>
@@ -4112,7 +4124,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="20"/>
@@ -4704,8 +4716,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4990,7 +5002,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="93" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D21" s="94"/>
     </row>
@@ -5062,7 +5074,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="92" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="9"/>
     </row>
@@ -5074,7 +5086,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="93" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="10"/>
     </row>
@@ -5086,33 +5098,47 @@
         <v>4</v>
       </c>
       <c r="C29" s="93" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A30" s="96" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C30" s="93" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="10"/>
+    <row r="31" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A31" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
+      <c r="C31" s="93" t="s">
+        <v>82</v>
+      </c>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
+    <row r="32" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="A32" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>4</v>
+      </c>
+      <c r="C32" s="93" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="94" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -5292,7 +5318,7 @@
       </c>
       <c r="B60" s="48">
         <f>SUM(B27:B59)</f>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C60" s="90" t="s">
         <v>37</v>
@@ -5342,16 +5368,17 @@
     <hyperlink ref="D6" r:id="rId1" display="https://clickup.com/fr-FR/blog/113716/outils-de-gestion-de-projet-en-cascade" xr:uid="{DA8F090E-F7C9-447F-A025-675A43AE436C}"/>
     <hyperlink ref="D17" r:id="rId2" display="https://www.nuget.org/packages/MySql.Data/" xr:uid="{D2F02347-FCC7-43CE-AD4D-A5D7157C9DB5}"/>
     <hyperlink ref="D18" r:id="rId3" display="https://www.w3schools.com/cs/cs_exceptions.php" xr:uid="{FA400CED-9B11-481C-8A43-4789B8DC1C63}"/>
+    <hyperlink ref="D32" r:id="rId4" xr:uid="{B8F39C6F-6383-418E-BEBD-67BD5B4D86C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId7" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+        <control shapeId="43009" r:id="rId8" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5370,7 +5397,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId7" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId8" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5378,26 +5405,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5618,26 +5625,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5654,4 +5662,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : class for displaying registered tasks done, automatic creation of labels in the panel for tasks
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D9A150-87D1-4ADC-A4E5-8BE84B7FC519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D144C9-4312-4982-813F-6094ABB061EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="3900" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6750" yWindow="2355" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
   <si>
     <t>Module :</t>
   </si>
@@ -599,9 +599,48 @@
     <t>https://prog101.com/exemples/csharp/chaines/compter-nombre-mot-dans-chaine.php</t>
   </si>
   <si>
-    <t>Recherche d'un moyen de compter le nombre de mot dans la tâche avant validation et ajout à la liste des tâches.
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Liens pour utilisation du menu contextuel: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://learn.microsoft.com/en-us/dotnet/api/system.windows.forms.contextmenustrip?view=windowsdesktop-9.0
+https://stackoverflow.com/questions/3631012/programmatically-adding-items-to-a-menu-strip</t>
+    </r>
+  </si>
+  <si>
+    <t>Suite des recherches /////////////////////////////////////////////// et test.</t>
+  </si>
+  <si>
+    <t>Recherche manière de récupérer l'identifiant de l'utilisateur en cours.</t>
+  </si>
+  <si>
+    <t>Recherche d'un moyen de compter le nombre de mots dans la tâche avant validation et ajout à la liste des tâches.
 Ajout de la tâche au tableau à vérifie.
 Affichage des tâches contenues dans la DB en cours.</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/65765089/how-to-display-username-when-you-logged-on-c-sharp-windows-forms-and-mysql-data</t>
+  </si>
+  <si>
+    <t>///</t>
+  </si>
+  <si>
+    <t>Finalisation de la classe "DisplayTasks" du modèle pour le renvoie d'une liste de tâche.
+Début création automatique de labels dans le panel de "TasksTodoPage".
+Recherches sur comment utiliser un menu contextuel depuis WindowsForm.</t>
   </si>
 </sst>
 </file>
@@ -3340,27 +3379,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3390,27 +3429,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3882,7 +3921,7 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -4716,8 +4755,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5134,34 +5173,62 @@
         <v>4</v>
       </c>
       <c r="C32" s="93" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D32" s="94" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="10"/>
+    <row r="33" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2">
+        <v>4</v>
+      </c>
+      <c r="C33" s="93" t="s">
+        <v>90</v>
+      </c>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="10"/>
+    <row r="34" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4</v>
+      </c>
+      <c r="C34" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="94" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="2">
+        <v>4</v>
+      </c>
+      <c r="C35" s="93" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A36" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2</v>
+      </c>
+      <c r="C36" s="93" t="s">
+        <v>89</v>
+      </c>
       <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5318,7 +5385,7 @@
       </c>
       <c r="B60" s="48">
         <f>SUM(B27:B59)</f>
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C60" s="90" t="s">
         <v>37</v>
@@ -5369,16 +5436,18 @@
     <hyperlink ref="D17" r:id="rId2" display="https://www.nuget.org/packages/MySql.Data/" xr:uid="{D2F02347-FCC7-43CE-AD4D-A5D7157C9DB5}"/>
     <hyperlink ref="D18" r:id="rId3" display="https://www.w3schools.com/cs/cs_exceptions.php" xr:uid="{FA400CED-9B11-481C-8A43-4789B8DC1C63}"/>
     <hyperlink ref="D32" r:id="rId4" xr:uid="{B8F39C6F-6383-418E-BEBD-67BD5B4D86C2}"/>
+    <hyperlink ref="D34" r:id="rId5" display="https://stackoverflow.com/questions/3631012/programmatically-adding-items-to-a-menu-strip" xr:uid="{F16E9BA4-87CA-423F-82EC-8FB4D3D3EC39}"/>
+    <hyperlink ref="D35" r:id="rId6" xr:uid="{F7BCC934-7D5C-4A0C-9789-AA5C98CEBAC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <drawing r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId8" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="43009" r:id="rId10" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5397,7 +5466,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId8" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId10" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5405,6 +5474,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5625,27 +5714,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5662,23 +5750,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : handle of all tasks in contextMenuStrip for TasksTodoPage.cs
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D144C9-4312-4982-813F-6094ABB061EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96232AF-C45A-4947-AAB8-A6A4609F91C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6750" yWindow="2355" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="4635" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
   <si>
     <t>Module :</t>
   </si>
@@ -642,6 +642,64 @@
 Début création automatique de labels dans le panel de "TasksTodoPage".
 Recherches sur comment utiliser un menu contextuel depuis WindowsForm.</t>
   </si>
+  <si>
+    <t>Récupération de l'id utilisateur okay.
+Affichage de toutes les tâches de l'utilisateur.
+Affichage du menu conceptuel avec ses fonctionnalités okay. Travail sur l'application de ses fonctionnalités.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Piste donnée par ChatGPT pour l'édition, convertir le label en textbox.
+Lien d'aide : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.developpez.net/forums/i1187847/dotnet/langages/vb-net/supprimer-button-winform/</t>
+    </r>
+  </si>
+  <si>
+    <t>Début code pour suppression de la tâche.
+Possibilité pour l'utilisateur d'éditer sa tâche okay.
+Recherche d'une méthode pour supprimer la tâche du panel et la mettre dans "TasksDonePage.cs" : tâche cachée, mais copie envoyée vers un autre form.
+Recherche moyen de détecter un "Enter" de l'utilisateur après l'édition de sa tâche.</t>
+  </si>
+  <si>
+    <t>"MessageBox" combiné à "DialogResult" pour permettre de supprimer ou non une tâche.
+Pour l'instant la tâche est seulement cachée suite à la décision de l'utilisateur.
+Problème avec l'ajout d'une tâche vers une autre page.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lien d'aide : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://learn.microsoft.com/en-us/dotnet/api/system.windows.forms.keyeventargs?view=windowsdesktop-9.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ChatGPT m'a aidé à l'adapté à mes besoins.
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -650,7 +708,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -785,6 +843,13 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF1B952A"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
       <name val="Century Gothic"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3379,27 +3444,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3429,27 +3494,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -4755,8 +4820,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5224,30 +5289,52 @@
         <v>31</v>
       </c>
       <c r="B36" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C36" s="93" t="s">
         <v>89</v>
       </c>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="10"/>
+    <row r="37" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="A37" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="2">
+        <v>4</v>
+      </c>
+      <c r="C37" s="93" t="s">
+        <v>91</v>
+      </c>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
+    <row r="38" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+      <c r="A38" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="2">
+        <v>4</v>
+      </c>
+      <c r="C38" s="93" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+      <c r="A39" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="2">
+        <v>4</v>
+      </c>
+      <c r="C39" s="93" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="93" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -5385,7 +5472,7 @@
       </c>
       <c r="B60" s="48">
         <f>SUM(B27:B59)</f>
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C60" s="90" t="s">
         <v>37</v>
@@ -5474,26 +5561,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5714,26 +5781,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5750,4 +5818,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : add of a task mark as done in TasksDonePage.cs
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96232AF-C45A-4947-AAB8-A6A4609F91C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4769A390-6FFA-4EF6-A1B6-BC1149732C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="4635" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="101">
   <si>
     <t>Module :</t>
   </si>
@@ -664,12 +664,6 @@
     </r>
   </si>
   <si>
-    <t>Début code pour suppression de la tâche.
-Possibilité pour l'utilisateur d'éditer sa tâche okay.
-Recherche d'une méthode pour supprimer la tâche du panel et la mettre dans "TasksDonePage.cs" : tâche cachée, mais copie envoyée vers un autre form.
-Recherche moyen de détecter un "Enter" de l'utilisateur après l'édition de sa tâche.</t>
-  </si>
-  <si>
     <t>"MessageBox" combiné à "DialogResult" pour permettre de supprimer ou non une tâche.
 Pour l'instant la tâche est seulement cachée suite à la décision de l'utilisateur.
 Problème avec l'ajout d'une tâche vers une autre page.</t>
@@ -696,9 +690,86 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-ChatGPT m'a aidé à l'adapté à mes besoins.
+ChatGPT m'a aidé à adapter le "keyevent" à mes besoins.
 </t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="9"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N.B. : pour toutes les tâches ci-dessous (et celles d'après liées au menu contextuel), j'ai travaillé sur un form séparé.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Début code pour suppression de la tâche.
+Possibilité pour l'utilisateur d'éditer sa tâche okay.
+Recherche d'une méthode pour supprimer la tâche du panel et la mettre dans "TasksDonePage.cs" : tâche cachée, mais copie envoyée vers un autre form.
+Recherche moyen de détecter un "Enter" de l'utilisateur après l'édition de sa tâche.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ajout d'une tâche vers une autre page okay, mais tâche pas affichée.
+Mise en place d'un mécanisme pour éviter que le menu contextuel ne s'ouvre alors qu'il est déjà ouvert.</t>
+  </si>
+  <si>
+    <t>Affichage de la tâche okay (dans l'environnment de test).
+Recherche manière de permettre à l'utilisateur de fermer le menu contextuel.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">P.S. : beaucoup d'erreurs lors de la regénération de la solution d'où mon retard.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Piste trouvée grâce au </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>conseil d'un camarade</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pour fermer le menu contextuel : utiliser une pictureBox.</t>
+    </r>
+  </si>
+  <si>
+    <t>Recherche pour pouvoir définir complètement une "PictureBox" manuellement.</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/fr-fr/dotnet/api/system.windows.forms.picturebox?view=windowsdesktop-8.0</t>
   </si>
 </sst>
 </file>
@@ -708,7 +779,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -854,6 +925,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="9"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF20B231"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1374,7 +1468,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1662,6 +1756,14 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1673,10 +1775,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF20B231"/>
       <color rgb="FF1B952A"/>
       <color rgb="FFFF0066"/>
       <color rgb="FF28663D"/>
-      <color rgb="FF20B231"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4820,8 +4922,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5308,7 +5410,7 @@
       </c>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="108" x14ac:dyDescent="0.25">
       <c r="A38" s="96" t="s">
         <v>31</v>
       </c>
@@ -5316,13 +5418,13 @@
         <v>4</v>
       </c>
       <c r="C38" s="93" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D38" s="93" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A39" s="96" t="s">
         <v>31</v>
       </c>
@@ -5330,35 +5432,61 @@
         <v>4</v>
       </c>
       <c r="C39" s="93" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="93" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="93" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="10"/>
+    </row>
+    <row r="40" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="2">
+        <v>4</v>
+      </c>
+      <c r="C40" s="93" t="s">
+        <v>96</v>
+      </c>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="10"/>
+    <row r="41" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A41" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="2">
+        <v>4</v>
+      </c>
+      <c r="C41" s="93" t="s">
+        <v>97</v>
+      </c>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
+    <row r="42" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42" s="2">
+        <v>4</v>
+      </c>
+      <c r="C42" s="102" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="103"/>
+    </row>
+    <row r="43" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2</v>
+      </c>
+      <c r="C43" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" s="94" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -5472,7 +5600,7 @@
       </c>
       <c r="B60" s="48">
         <f>SUM(B27:B59)</f>
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C60" s="90" t="s">
         <v>37</v>
@@ -5525,16 +5653,17 @@
     <hyperlink ref="D32" r:id="rId4" xr:uid="{B8F39C6F-6383-418E-BEBD-67BD5B4D86C2}"/>
     <hyperlink ref="D34" r:id="rId5" display="https://stackoverflow.com/questions/3631012/programmatically-adding-items-to-a-menu-strip" xr:uid="{F16E9BA4-87CA-423F-82EC-8FB4D3D3EC39}"/>
     <hyperlink ref="D35" r:id="rId6" xr:uid="{F7BCC934-7D5C-4A0C-9789-AA5C98CEBAC2}"/>
+    <hyperlink ref="D43" r:id="rId7" xr:uid="{E38CD9D3-B9BD-4BD4-B5BA-9A3F11D514B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
-  <drawing r:id="rId8"/>
-  <legacyDrawing r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <drawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId10" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+        <control shapeId="43009" r:id="rId11" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5553,7 +5682,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId10" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId11" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
feat : start of management of a close button on TasksTodoPage.cs's menu
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4769A390-6FFA-4EF6-A1B6-BC1149732C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C910C6D-7FF1-4EA0-A464-0C4E446B4A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="105">
   <si>
     <t>Module :</t>
   </si>
@@ -766,10 +766,26 @@
     </r>
   </si>
   <si>
-    <t>Recherche pour pouvoir définir complètement une "PictureBox" manuellement.</t>
-  </si>
-  <si>
     <t>https://learn.microsoft.com/fr-fr/dotnet/api/system.windows.forms.picturebox?view=windowsdesktop-8.0</t>
+  </si>
+  <si>
+    <t>Recherche pour définir une "PictureBox" manuellement, abandon de cette méthode pour lier le bouton au menu. Difficulté à gérer la fermeture du menu.</t>
+  </si>
+  <si>
+    <t>Réflexion pour afficher les tâches.
+Début contrôle du mot de passe d'un nouveau utilisateur.</t>
+  </si>
+  <si>
+    <t>///
+Pourquoi ? - Je fais d'autres choses en parralèle qui ne sont pas liées à cet exercice</t>
+  </si>
+  <si>
+    <t>///
+Pourquoi ? - ///</t>
+  </si>
+  <si>
+    <t>///
+10 mn</t>
   </si>
 </sst>
 </file>
@@ -1746,16 +1762,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1764,6 +1770,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2701,10 +2717,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="99"/>
+      <c r="C19" s="101"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -3546,27 +3562,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3596,27 +3612,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3655,7 +3671,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="102" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3664,7 +3680,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="101"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -4920,10 +4936,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5469,47 +5485,71 @@
       <c r="B42" s="2">
         <v>4</v>
       </c>
-      <c r="C42" s="102" t="s">
+      <c r="C42" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="103"/>
+      <c r="D42" s="99"/>
     </row>
     <row r="43" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A43" s="96" t="s">
         <v>31</v>
       </c>
       <c r="B43" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C43" s="93" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="D43" s="94" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="10"/>
+    </row>
+    <row r="44" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A44" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="2">
+        <v>4</v>
+      </c>
+      <c r="C44" s="93" t="s">
+        <v>101</v>
+      </c>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="10"/>
+    <row r="45" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A45" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="2">
+        <v>4</v>
+      </c>
+      <c r="C45" s="93" t="s">
+        <v>102</v>
+      </c>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="10"/>
+    <row r="46" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A46" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="2">
+        <v>4</v>
+      </c>
+      <c r="C46" s="93" t="s">
+        <v>103</v>
+      </c>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="10"/>
+    <row r="47" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A47" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="2">
+        <v>4</v>
+      </c>
+      <c r="C47" s="93" t="s">
+        <v>104</v>
+      </c>
       <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5518,131 +5558,197 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
-    </row>
-    <row r="59" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="34"/>
-      <c r="I59" s="20"/>
-    </row>
-    <row r="60" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="48" t="s">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20"/>
+      <c r="I69" s="20"/>
+    </row>
+    <row r="70" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="33"/>
+      <c r="H70" s="34"/>
+      <c r="I70" s="20"/>
+    </row>
+    <row r="71" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B60" s="48">
-        <f>SUM(B27:B59)</f>
-        <v>66</v>
-      </c>
-      <c r="C60" s="90" t="s">
+      <c r="B71" s="48">
+        <f>SUM(B27:B70)</f>
+        <v>84</v>
+      </c>
+      <c r="C71" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D60" s="49"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-    </row>
-    <row r="61" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A61" s="50"/>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="91" t="s">
+      <c r="D71" s="49"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20"/>
+      <c r="I71" s="20"/>
+    </row>
+    <row r="72" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A72" s="50"/>
+      <c r="B72" s="50"/>
+      <c r="C72" s="50"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="20"/>
+      <c r="I72" s="20"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B27:B59 B3:B22" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B27:B70 B3:B22" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B60" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B71" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27:A59 A3:A22" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27:A70 A3:A22" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -5690,6 +5796,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5910,27 +6036,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5947,23 +6072,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : control of new user data
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C910C6D-7FF1-4EA0-A464-0C4E446B4A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB29F0E-ECDB-47E5-AB55-44313750EAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8550" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="109">
   <si>
     <t>Module :</t>
   </si>
@@ -777,15 +777,30 @@
   </si>
   <si>
     <t>///
+Pourquoi ? - ///</t>
+  </si>
+  <si>
+    <t>/// (utilisation de ChatGPT infructueuse.)
 Pourquoi ? - Je fais d'autres choses en parralèle qui ne sont pas liées à cet exercice</t>
   </si>
   <si>
-    <t>///
-Pourquoi ? - ///</t>
-  </si>
-  <si>
-    <t>///
-10 mn</t>
+    <t>Après relecture d'anciens codes, problème n° 9 résolu.</t>
+  </si>
+  <si>
+    <t>https://www.webdevtutor.net/blog/c-sharp-mysql-parameterized-query</t>
+  </si>
+  <si>
+    <t>Erreur n° 13 (index hors limite).
+Recherche méthode pour sécuriser les requêtes MySQL (aucune application n'a été faite).</t>
+  </si>
+  <si>
+    <t>https://www.developpez.net/forums/d275096/dotnet/langages/csharp/expression-reguliere-verifiaction-d-passe/</t>
+  </si>
+  <si>
+    <t>Résolution de l'erreur n° 13.
+Vérification disponibilité d'un nom d'utilisateur okay.
+Vérification de la longueur et du contenu du mot de passe (miniscules, majuscules, caractères spéciaux, chiffres) okay.
+Suppression des paramètres du constructeur de "HomePage.cs" et des assignations de propriétés (image et texte) pour partager le logo et le nom de l'application via le "Controller.cs".</t>
   </si>
 </sst>
 </file>
@@ -1484,7 +1499,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1780,6 +1795,10 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3562,27 +3581,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3612,27 +3631,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -4938,8 +4957,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5524,7 +5543,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="93" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D45" s="10"/>
     </row>
@@ -5536,7 +5555,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D46" s="10"/>
     </row>
@@ -5548,32 +5567,56 @@
         <v>4</v>
       </c>
       <c r="C47" s="93" t="s">
+        <v>89</v>
+      </c>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A48" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="2">
+        <v>4</v>
+      </c>
+      <c r="C48" s="93" t="s">
         <v>104</v>
       </c>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="10"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
+    <row r="49" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A49" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="2">
+        <v>4</v>
+      </c>
+      <c r="C49" s="104" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="94" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="2">
+        <v>4</v>
+      </c>
+      <c r="C50" s="93" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="94" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="10"/>
+      <c r="C51" s="10">
+        <v>10</v>
+      </c>
       <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -5706,7 +5749,7 @@
       </c>
       <c r="B71" s="48">
         <f>SUM(B27:B70)</f>
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C71" s="90" t="s">
         <v>37</v>
@@ -5760,16 +5803,18 @@
     <hyperlink ref="D34" r:id="rId5" display="https://stackoverflow.com/questions/3631012/programmatically-adding-items-to-a-menu-strip" xr:uid="{F16E9BA4-87CA-423F-82EC-8FB4D3D3EC39}"/>
     <hyperlink ref="D35" r:id="rId6" xr:uid="{F7BCC934-7D5C-4A0C-9789-AA5C98CEBAC2}"/>
     <hyperlink ref="D43" r:id="rId7" xr:uid="{E38CD9D3-B9BD-4BD4-B5BA-9A3F11D514B5}"/>
+    <hyperlink ref="D49" r:id="rId8" xr:uid="{0700A3BE-582B-4A90-BE08-860238EE2B7E}"/>
+    <hyperlink ref="D50" r:id="rId9" xr:uid="{0E42211F-349E-45E8-B178-C0DD4A989548}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
-  <drawing r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <drawing r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId11" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+        <control shapeId="43009" r:id="rId13" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5788,7 +5833,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId11" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId13" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5796,26 +5841,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -6036,26 +6061,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6072,4 +6098,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
style : resquests secure
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB29F0E-ECDB-47E5-AB55-44313750EAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A4D189-054F-4ED6-A8B8-BF9AC25195CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8550" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4095" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="113">
   <si>
     <t>Module :</t>
   </si>
@@ -802,6 +802,43 @@
 Vérification de la longueur et du contenu du mot de passe (miniscules, majuscules, caractères spéciaux, chiffres) okay.
 Suppression des paramètres du constructeur de "HomePage.cs" et des assignations de propriétés (image et texte) pour partager le logo et le nom de l'application via le "Controller.cs".</t>
   </si>
+  <si>
+    <t>Etablissement de la classe "CreateUser" pour ajouter un nouvel utilisateur dans la base de données.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lien d'aide pour le code de la classe ajout de données en C#, modification des classes update et delete en conséquence (dataReader pas adapté) : </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://zetcode.com/csharp/mysql/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Requêtes sécurisées. </t>
+  </si>
+  <si>
+    <t>20
+Hachage du mot de pase.
+Fermer la connexion à la DB.</t>
+  </si>
 </sst>
 </file>
 
@@ -810,7 +847,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -979,6 +1016,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1785,20 +1830,20 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2736,10 +2781,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="101"/>
+      <c r="C19" s="102"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -3581,27 +3626,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3631,27 +3676,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3690,7 +3735,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="103" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3699,7 +3744,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="103"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -4123,7 +4168,7 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -4957,8 +5002,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5590,7 +5635,7 @@
       <c r="B49" s="2">
         <v>4</v>
       </c>
-      <c r="C49" s="104" t="s">
+      <c r="C49" s="100" t="s">
         <v>106</v>
       </c>
       <c r="D49" s="94" t="s">
@@ -5599,7 +5644,7 @@
     </row>
     <row r="50" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A50" s="96" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B50" s="2">
         <v>4</v>
@@ -5611,24 +5656,42 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="10">
-        <v>10</v>
-      </c>
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="10"/>
+    <row r="51" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+      <c r="A51" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" s="2">
+        <v>4</v>
+      </c>
+      <c r="C51" s="93" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="93" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A52" s="96" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="2">
+        <v>4</v>
+      </c>
+      <c r="C52" s="93" t="s">
+        <v>111</v>
+      </c>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="10"/>
+    <row r="53" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="96" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="2">
+        <v>4</v>
+      </c>
+      <c r="C53" s="93" t="s">
+        <v>112</v>
+      </c>
       <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -5749,7 +5812,7 @@
       </c>
       <c r="B71" s="48">
         <f>SUM(B27:B70)</f>
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C71" s="90" t="s">
         <v>37</v>
@@ -5841,6 +5904,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -6061,27 +6144,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6098,23 +6180,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : add of a task in database; fix : introduction of the task's boolean variable in structural models
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A4D189-054F-4ED6-A8B8-BF9AC25195CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A303F62-C672-4A41-A850-B1077DACE575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4095" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="120">
   <si>
     <t>Module :</t>
   </si>
@@ -835,9 +835,71 @@
     <t xml:space="preserve">Requêtes sécurisées. </t>
   </si>
   <si>
-    <t>20
-Hachage du mot de pase.
+    <t>Travail supplémentaire</t>
+  </si>
+  <si>
+    <t>Hachage du mot de pase.
 Fermer la connexion à la DB.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Liens utilisés en plus de ChatGPT : 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.w3schools.com/mysql/mysql_insert_into_select.asp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.mysqltutorial.org/mysql-basics/mysql-insert-into-select/</t>
+    </r>
+  </si>
+  <si>
+    <t>Recherche solution pour la requête permettant d'ajouter des tâches.
+Utilisation de :
+"INSERT INTO … SELECT … WHERE...",
+"INSERT INTO … VALUES((SELECT...),(SELECT...), ...)".</t>
+  </si>
+  <si>
+    <t>Découverte du problème : la condition de mon where était pour un user_id à 1. Et il n'y en avait pas. Retour sur ma version simplifiée.
+Ajout d'une tâche dans la base de données okay.</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/748062/return-multiple-values-to-a-method-caller</t>
+  </si>
+  <si>
+    <t>Modification des modèles (MCD, MLD, MPD) pour introduire une variable booléan pour savoir si une tâche a été faite.
+Recherche méthode pour retourner deux valeurs et deux types de variables. 
+-&gt; Simplification par le contrôle de l'état de la tâche dans le modèle avant de l'ajouter dans la liste des tâches à retourner.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalisation de l'ajout d'un utilisateur à la base de données.
+</t>
   </si>
 </sst>
 </file>
@@ -847,7 +909,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
@@ -1024,6 +1086,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1105,7 +1176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1534,6 +1605,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1544,7 +1639,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1844,6 +1939,18 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -5002,8 +5109,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5682,21 +5789,25 @@
       </c>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A53" s="96" t="s">
         <v>35</v>
       </c>
       <c r="B53" s="2">
+        <v>3</v>
+      </c>
+      <c r="C53" s="93" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="10"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="2">
         <v>4</v>
       </c>
-      <c r="C53" s="93" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
     </row>
@@ -5712,34 +5823,64 @@
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="10"/>
+    <row r="57" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="105" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="106"/>
+      <c r="C57" s="106"/>
+      <c r="D57" s="107"/>
+    </row>
+    <row r="58" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+      <c r="A58" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="2">
+        <v>4</v>
+      </c>
+      <c r="C58" s="93" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="93" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="2">
+        <v>4</v>
+      </c>
+      <c r="C59" s="93" t="s">
+        <v>116</v>
+      </c>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="10"/>
+    <row r="60" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="2">
+        <v>4</v>
+      </c>
+      <c r="C60" s="93" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" s="94" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="2">
+        <v>2</v>
+      </c>
+      <c r="C61" s="93" t="s">
+        <v>119</v>
+      </c>
       <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -5775,7 +5916,7 @@
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="10"/>
+      <c r="C67" s="93"/>
       <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -5812,7 +5953,7 @@
       </c>
       <c r="B71" s="48">
         <f>SUM(B27:B70)</f>
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C71" s="90" t="s">
         <v>37</v>
@@ -5846,8 +5987,11 @@
       <c r="I73" s="20"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A57:D57"/>
+  </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B27:B70 B3:B22" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B70" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B71" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
@@ -5868,16 +6012,17 @@
     <hyperlink ref="D43" r:id="rId7" xr:uid="{E38CD9D3-B9BD-4BD4-B5BA-9A3F11D514B5}"/>
     <hyperlink ref="D49" r:id="rId8" xr:uid="{0700A3BE-582B-4A90-BE08-860238EE2B7E}"/>
     <hyperlink ref="D50" r:id="rId9" xr:uid="{0E42211F-349E-45E8-B178-C0DD4A989548}"/>
+    <hyperlink ref="D60" r:id="rId10" xr:uid="{9D7FDC9D-EF01-48DE-80E0-1F69C20D4B4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
-  <drawing r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <drawing r:id="rId12"/>
+  <legacyDrawing r:id="rId13"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId13" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+        <control shapeId="43009" r:id="rId14" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5896,7 +6041,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId13" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId14" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
perf : suppression of ManageTasks class; feat : display of one task; fix : suppression of a task in the tasks list
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A303F62-C672-4A41-A850-B1077DACE575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D40419F-7F9B-440F-9D4E-A69C2D291C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4905" yWindow="2970" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="124">
   <si>
     <t>Module :</t>
   </si>
@@ -898,8 +898,24 @@
 -&gt; Simplification par le contrôle de l'état de la tâche dans le modèle avant de l'ajouter dans la liste des tâches à retourner.</t>
   </si>
   <si>
-    <t xml:space="preserve">Finalisation de l'ajout d'un utilisateur à la base de données.
-</t>
+    <t>https://waytolearnx.com/2019/09/comment-extraire-des-nombres-dune-chaine-de-caracteres-en-csharp.html</t>
+  </si>
+  <si>
+    <t>Finalisation de l'ajout d'un utilisateur à la base de données.
+Code pour afficher les tâches faites (reprise du code de "TasksTodoPage.cs"). 
+Connexion au contrôleur pour une suppression définitive d'une tâche.
+Début code pour supprimer une tâche de la liste des tâches.</t>
+  </si>
+  <si>
+    <t>Insertion de données de test pour les tâches utilisateurs (utilisation de ChatGPT).
+Test affichage des tâches mais erreur de compilation.</t>
+  </si>
+  <si>
+    <t>Suite code pour supprimer une tâche de la liste des tâches.</t>
+  </si>
+  <si>
+    <t>Affichage d'une seule tâche.
+Problème lors de la suppression d'une tâche (erreur n° 17).</t>
   </si>
 </sst>
 </file>
@@ -3733,27 +3749,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3783,27 +3799,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5107,10 +5123,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5871,34 +5887,50 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="2">
+        <v>4</v>
+      </c>
+      <c r="C61" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="94" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A62" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="2">
-        <v>2</v>
-      </c>
-      <c r="C61" s="93" t="s">
-        <v>119</v>
-      </c>
-      <c r="D61" s="10"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="10"/>
+      <c r="B62" s="2">
+        <v>4</v>
+      </c>
+      <c r="C62" s="93" t="s">
+        <v>121</v>
+      </c>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="10"/>
+    <row r="63" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A63" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="2">
+        <v>4</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>122</v>
+      </c>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="10"/>
+      <c r="C64" s="93" t="s">
+        <v>123</v>
+      </c>
       <c r="D64" s="10"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -5916,7 +5948,7 @@
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="93"/>
+      <c r="C67" s="10"/>
       <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -5930,75 +5962,105 @@
       <c r="B69" s="2"/>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="20"/>
-      <c r="H69" s="20"/>
-      <c r="I69" s="20"/>
-    </row>
-    <row r="70" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="33"/>
-      <c r="H70" s="34"/>
-      <c r="I70" s="20"/>
-    </row>
-    <row r="71" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="48" t="s">
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="93"/>
+      <c r="D72" s="10"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="20"/>
+    </row>
+    <row r="75" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="34"/>
+      <c r="I75" s="20"/>
+    </row>
+    <row r="76" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B71" s="48">
-        <f>SUM(B27:B70)</f>
-        <v>125</v>
-      </c>
-      <c r="C71" s="90" t="s">
+      <c r="B76" s="48">
+        <f>SUM(B27:B75)</f>
+        <v>135</v>
+      </c>
+      <c r="C76" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D71" s="49"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="20"/>
-      <c r="H71" s="20"/>
-      <c r="I71" s="20"/>
-    </row>
-    <row r="72" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A72" s="50"/>
-      <c r="B72" s="50"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="G72" s="20"/>
-      <c r="H72" s="20"/>
-      <c r="I72" s="20"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="91" t="s">
+      <c r="D76" s="49"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
+    </row>
+    <row r="77" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A77" s="50"/>
+      <c r="B77" s="50"/>
+      <c r="C77" s="50"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="20"/>
+      <c r="I77" s="20"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="G73" s="20"/>
-      <c r="H73" s="20"/>
-      <c r="I73" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B70" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B75" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B71" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B76" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27:A70 A3:A22" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27:A75 A3:A22" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -6013,16 +6075,17 @@
     <hyperlink ref="D49" r:id="rId8" xr:uid="{0700A3BE-582B-4A90-BE08-860238EE2B7E}"/>
     <hyperlink ref="D50" r:id="rId9" xr:uid="{0E42211F-349E-45E8-B178-C0DD4A989548}"/>
     <hyperlink ref="D60" r:id="rId10" xr:uid="{9D7FDC9D-EF01-48DE-80E0-1F69C20D4B4E}"/>
+    <hyperlink ref="D61" r:id="rId11" xr:uid="{D9DF375C-7B06-4F91-B7AB-C5090DB2E41D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
-  <drawing r:id="rId12"/>
-  <legacyDrawing r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <drawing r:id="rId13"/>
+  <legacyDrawing r:id="rId14"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId14" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+        <control shapeId="43009" r:id="rId15" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -6041,7 +6104,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId14" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId15" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -6049,26 +6112,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -6289,26 +6332,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6325,4 +6369,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : start hash password; docs : source, work managemnet criticism
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D40419F-7F9B-440F-9D4E-A69C2D291C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC5A099-B84B-4F7D-AAA3-3E288B94447C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4905" yWindow="2970" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="3855" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="132">
   <si>
     <t>Module :</t>
   </si>
@@ -838,10 +838,6 @@
     <t>Travail supplémentaire</t>
   </si>
   <si>
-    <t>Hachage du mot de pase.
-Fermer la connexion à la DB.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Liens utilisés en plus de ChatGPT : 
 </t>
@@ -911,11 +907,45 @@
 Test affichage des tâches mais erreur de compilation.</t>
   </si>
   <si>
-    <t>Suite code pour supprimer une tâche de la liste des tâches.</t>
-  </si>
-  <si>
-    <t>Affichage d'une seule tâche.
+    <t>Suite code pour supprimer une tâche de la liste des tâches.
+Affichage d'une seule tâche.
 Problème lors de la suppression d'une tâche (erreur n° 17).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage de toutes les tâches.
+</t>
+  </si>
+  <si>
+    <t>Correction de l'erreur n° 17 (test de la solution sur internet à cause d'une erreur de compilation).</t>
+  </si>
+  <si>
+    <t>???Hachage du mot de pase.
+Fermer la connexion à la DB.</t>
+  </si>
+  <si>
+    <t>Nettoyage du code et commentaires.
+Finalisation du code pour la modification de l'intitulé d'une tâche.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Présentation stage post CFC M. Garraux. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code commenté.
+</t>
+  </si>
+  <si>
+    <t>C# Language Tutorial =&gt; Password Hashing</t>
+  </si>
+  <si>
+    <t>Recherche solution pour réduire problèmes de compilation (en vain).
+Recherche hashage du mot de passe avant sauvegarde DB.</t>
+  </si>
+  <si>
+    <t>Documentation (source et critique).</t>
+  </si>
+  <si>
+    <t>Suite code pour hachage du mot de passe (pas terminé).
+Début documentation à l'aide de la grille d'évaluation.</t>
   </si>
 </sst>
 </file>
@@ -1655,7 +1685,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1945,6 +1975,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2904,10 +2938,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="101" t="s">
+      <c r="B19" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="102"/>
+      <c r="C19" s="104"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -3858,7 +3892,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="105" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3867,7 +3901,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="104"/>
+      <c r="B4" s="106"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -4291,8 +4325,8 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5123,10 +5157,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5813,7 +5847,7 @@
         <v>3</v>
       </c>
       <c r="C53" s="93" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="D53" s="10"/>
     </row>
@@ -5840,12 +5874,12 @@
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="105" t="s">
+      <c r="A57" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="106"/>
-      <c r="C57" s="106"/>
-      <c r="D57" s="107"/>
+      <c r="B57" s="108"/>
+      <c r="C57" s="108"/>
+      <c r="D57" s="109"/>
     </row>
     <row r="58" spans="1:4" ht="81" x14ac:dyDescent="0.25">
       <c r="A58" s="96" t="s">
@@ -5855,10 +5889,10 @@
         <v>4</v>
       </c>
       <c r="C58" s="93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D58" s="93" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
@@ -5869,7 +5903,7 @@
         <v>4</v>
       </c>
       <c r="C59" s="93" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D59" s="10"/>
     </row>
@@ -5881,10 +5915,10 @@
         <v>4</v>
       </c>
       <c r="C60" s="93" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D60" s="94" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="54" x14ac:dyDescent="0.25">
@@ -5895,90 +5929,138 @@
         <v>4</v>
       </c>
       <c r="C61" s="93" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D61" s="94" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="96" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62" s="2">
         <v>4</v>
       </c>
       <c r="C62" s="93" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A63" s="96" t="s">
         <v>31</v>
       </c>
       <c r="B63" s="2">
         <v>4</v>
       </c>
-      <c r="C63" s="29" t="s">
+      <c r="C63" s="101" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" s="10"/>
+    </row>
+    <row r="64" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A64" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="2">
+        <v>4</v>
+      </c>
+      <c r="C64" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="93" t="s">
+      <c r="D64" s="10"/>
+    </row>
+    <row r="65" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A65" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="2">
+        <v>4</v>
+      </c>
+      <c r="C65" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="D64" s="10"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="10"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="10"/>
+    <row r="66" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A66" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="2">
+        <v>4</v>
+      </c>
+      <c r="C66" s="93" t="s">
+        <v>125</v>
+      </c>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="10"/>
+    <row r="67" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A67" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="2">
+        <v>2</v>
+      </c>
+      <c r="C67" s="93" t="s">
+        <v>127</v>
+      </c>
       <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="10"/>
+      <c r="A68" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="2">
+        <v>2</v>
+      </c>
+      <c r="C68" s="93" t="s">
+        <v>126</v>
+      </c>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="10"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="10"/>
+    <row r="69" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="2">
+        <v>4</v>
+      </c>
+      <c r="C69" s="93" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="102" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" s="2">
+        <v>4</v>
+      </c>
+      <c r="C70" s="93" t="s">
+        <v>131</v>
+      </c>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="10"/>
+    <row r="71" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" s="2">
+        <v>4</v>
+      </c>
+      <c r="C71" s="93" t="s">
+        <v>130</v>
+      </c>
       <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2"/>
-      <c r="C72" s="93"/>
+      <c r="C72" s="10"/>
       <c r="D72" s="10"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -5992,75 +6074,111 @@
       <c r="B74" s="2"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="20"/>
-      <c r="H74" s="20"/>
-      <c r="I74" s="20"/>
-    </row>
-    <row r="75" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="32"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="34"/>
-      <c r="I75" s="20"/>
-    </row>
-    <row r="76" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="48" t="s">
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="93"/>
+      <c r="D78" s="10"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="20"/>
+    </row>
+    <row r="81" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="32"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="34"/>
+      <c r="I81" s="20"/>
+    </row>
+    <row r="82" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B76" s="48">
-        <f>SUM(B27:B75)</f>
-        <v>135</v>
-      </c>
-      <c r="C76" s="90" t="s">
+      <c r="B82" s="48">
+        <f>SUM(B27:B81)</f>
+        <v>163</v>
+      </c>
+      <c r="C82" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D76" s="49"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="20"/>
-      <c r="H76" s="20"/>
-      <c r="I76" s="20"/>
-    </row>
-    <row r="77" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A77" s="50"/>
-      <c r="B77" s="50"/>
-      <c r="C77" s="50"/>
-      <c r="D77" s="50"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="20"/>
-      <c r="H77" s="20"/>
-      <c r="I77" s="20"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="91" t="s">
+      <c r="D82" s="49"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="20"/>
+    </row>
+    <row r="83" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A83" s="50"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="50"/>
+      <c r="D83" s="50"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="20"/>
-      <c r="H78" s="20"/>
-      <c r="I78" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B75" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B81" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B76" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B82" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27:A75 A3:A22" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A81" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -6076,16 +6194,17 @@
     <hyperlink ref="D50" r:id="rId9" xr:uid="{0E42211F-349E-45E8-B178-C0DD4A989548}"/>
     <hyperlink ref="D60" r:id="rId10" xr:uid="{9D7FDC9D-EF01-48DE-80E0-1F69C20D4B4E}"/>
     <hyperlink ref="D61" r:id="rId11" xr:uid="{D9DF375C-7B06-4F91-B7AB-C5090DB2E41D}"/>
+    <hyperlink ref="D69" r:id="rId12" display="https://riptutorial.com/csharp/example/20103/password-hashing" xr:uid="{08AF6903-8615-445A-9B9E-07607C69C38F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
-  <drawing r:id="rId13"/>
-  <legacyDrawing r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <drawing r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId15" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+        <control shapeId="43009" r:id="rId16" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -6104,7 +6223,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId15" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId16" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
docs : introduction, finalization of sources, schedule chart
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC5A099-B84B-4F7D-AAA3-3E288B94447C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74406DE-783D-4701-876A-E884D89F4FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3855" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Planning" sheetId="155" r:id="rId5"/>
     <sheet name="achievementWeek" sheetId="154" state="hidden" r:id="rId6"/>
     <sheet name="JNLTRAV" sheetId="156" r:id="rId7"/>
+    <sheet name="Graphique-Planning" sheetId="157" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="datDateBegin">Donnees!$C$9</definedName>
@@ -54,8 +55,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="140">
   <si>
     <t>Module :</t>
   </si>
@@ -941,11 +964,53 @@
 Recherche hashage du mot de passe avant sauvegarde DB.</t>
   </si>
   <si>
-    <t>Documentation (source et critique).</t>
-  </si>
-  <si>
     <t>Suite code pour hachage du mot de passe (pas terminé).
 Début documentation à l'aide de la grille d'évaluation.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Lien d'aide pour gérer la communication entre fenêtres :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://www.youtube.com/watch?v=qFyRtrv-QDY</t>
+    </r>
+  </si>
+  <si>
+    <t>Documentation (suite et fin des sources).</t>
+  </si>
+  <si>
+    <t>Documentation (début de l'introduction).</t>
+  </si>
+  <si>
+    <t>Documentation (suite et fin de l'introduction).</t>
+  </si>
+  <si>
+    <t>Documentation (début des sources et critique, entête et pied de page).</t>
+  </si>
+  <si>
+    <t>Tâches</t>
+  </si>
+  <si>
+    <t>Nb de quart d'heure</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Documentation - page de titre, graphique du planning.</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1207,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1221,6 +1286,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -1685,7 +1756,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1998,6 +2069,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2055,6 +2130,879 @@
 
 <file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphique-Planning'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nb de quart d'heure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphique-Planning'!$A$2:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>Préparation au projet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Création des interfaces graphiques</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Implémentation de la base de données</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Relation base de données - application</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Absence - Imprévus</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Fonctionnalités du programme</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Documentation et modèles structurants</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Autres points techniques</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tests</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Absence - Imprévus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphique-Planning'!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AADD-47D6-A650-3AFF3523BF3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1724095039"/>
+        <c:axId val="1463892639"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1724095039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1463892639"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1463892639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1724095039"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2488,6 +3436,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ABA34B8-1581-EA06-9EBB-E8B18417F662}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ThèmeGGZExcel">
   <a:themeElements>
@@ -3783,27 +4772,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3833,27 +4822,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -4326,7 +5315,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5159,8 +6148,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5289,7 +6278,9 @@
       <c r="C9" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="94"/>
+      <c r="D9" s="94" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="10" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -5960,7 +6951,7 @@
       <c r="D63" s="10"/>
     </row>
     <row r="64" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A64" s="96" t="s">
+      <c r="A64" s="110" t="s">
         <v>31</v>
       </c>
       <c r="B64" s="2">
@@ -6041,7 +7032,7 @@
         <v>4</v>
       </c>
       <c r="C70" s="93" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D70" s="10"/>
     </row>
@@ -6053,32 +7044,56 @@
         <v>4</v>
       </c>
       <c r="C71" s="93" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="10"/>
+    <row r="72" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A72" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" s="2">
+        <v>4</v>
+      </c>
+      <c r="C72" s="93" t="s">
+        <v>133</v>
+      </c>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="10"/>
+    <row r="73" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A73" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" s="2">
+        <v>4</v>
+      </c>
+      <c r="C73" s="93" t="s">
+        <v>132</v>
+      </c>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="10"/>
+    <row r="74" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A74" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="B74" s="2">
+        <v>4</v>
+      </c>
+      <c r="C74" s="93" t="s">
+        <v>134</v>
+      </c>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="10"/>
+    <row r="75" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A75" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" s="2">
+        <v>2</v>
+      </c>
+      <c r="C75" s="93" t="s">
+        <v>139</v>
+      </c>
       <c r="D75" s="10"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -6133,7 +7148,7 @@
       </c>
       <c r="B82" s="48">
         <f>SUM(B27:B81)</f>
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="C82" s="90" t="s">
         <v>37</v>
@@ -6195,16 +7210,17 @@
     <hyperlink ref="D60" r:id="rId10" xr:uid="{9D7FDC9D-EF01-48DE-80E0-1F69C20D4B4E}"/>
     <hyperlink ref="D61" r:id="rId11" xr:uid="{D9DF375C-7B06-4F91-B7AB-C5090DB2E41D}"/>
     <hyperlink ref="D69" r:id="rId12" display="https://riptutorial.com/csharp/example/20103/password-hashing" xr:uid="{08AF6903-8615-445A-9B9E-07607C69C38F}"/>
+    <hyperlink ref="D9" r:id="rId13" display="https://www.youtube.com/watch?v=qFyRtrv-QDY" xr:uid="{91D49F7A-DAFE-41D3-851F-FF0E4C6B445F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
-  <drawing r:id="rId14"/>
-  <legacyDrawing r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <drawing r:id="rId15"/>
+  <legacyDrawing r:id="rId16"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId16" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="43009" r:id="rId17" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -6223,14 +7239,161 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId16" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId17" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3226A54-7399-49BB-B371-B772FF320D3A}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:B7">Planning!A3:B8</f>
+        <v>Préparation au projet</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <v>Création des interfaces graphiques</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <v>Implémentation de la base de données</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <v>Relation base de données - application</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <v>Absence - Imprévus</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="str" cm="1">
+        <f t="array" ref="A8:B12">Planning!A17:B21</f>
+        <v>Fonctionnalités du programme</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <v>Documentation et modèles structurants</v>
+      </c>
+      <c r="B9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <v>Autres points techniques</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <v>Tests</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <v>Absence - Imprévus</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B2:B12)</f>
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -6451,27 +7614,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6488,23 +7650,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs : documentation final stages
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74406DE-783D-4701-876A-E884D89F4FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65508A48-2834-4313-A0C6-D11563AE78CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="achievementWeek" sheetId="154" state="hidden" r:id="rId6"/>
     <sheet name="JNLTRAV" sheetId="156" r:id="rId7"/>
     <sheet name="Graphique-Planning" sheetId="157" r:id="rId8"/>
+    <sheet name="Graphique-JNLTRAV" sheetId="158" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="datDateBegin">Donnees!$C$9</definedName>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="142">
   <si>
     <t>Module :</t>
   </si>
@@ -650,11 +651,6 @@
     <t>Recherche manière de récupérer l'identifiant de l'utilisateur en cours.</t>
   </si>
   <si>
-    <t>Recherche d'un moyen de compter le nombre de mots dans la tâche avant validation et ajout à la liste des tâches.
-Ajout de la tâche au tableau à vérifie.
-Affichage des tâches contenues dans la DB en cours.</t>
-  </si>
-  <si>
     <t>https://stackoverflow.com/questions/65765089/how-to-display-username-when-you-logged-on-c-sharp-windows-forms-and-mysql-data</t>
   </si>
   <si>
@@ -1011,6 +1007,17 @@
   </si>
   <si>
     <t>Documentation - page de titre, graphique du planning.</t>
+  </si>
+  <si>
+    <t>Recherche d'un moyen de compter le nombre de mots dans la tâche avant validation et ajout à la liste des tâches.
+Ajout de la tâche au tableau à vérifier.
+Affichage des tâches contenues dans la DB en cours.</t>
+  </si>
+  <si>
+    <t>Mise au propre, conclusion, graphique du journal de travail.</t>
+  </si>
+  <si>
+    <t>Mise au propre.</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1286,12 +1293,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="36">
     <border>
@@ -1756,7 +1757,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2072,10 +2073,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2147,6 +2144,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Répartition</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 1/4 d'heure planning</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2460,6 +2487,700 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CH"/>
+              <a:t>Répartition</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CH" baseline="0"/>
+              <a:t> 1/4 d'heure JNLTRAV</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CH"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphique-JNLTRAV'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nb de quart d'heure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphique-JNLTRAV'!$A$2:$A$68</c:f>
+              <c:strCache>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>Absence - Imprévus</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Préparation au projet</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Préparation au projet</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Préparation au projet</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Préparation au projet</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Création des interfaces graphiques</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Création des interfaces graphiques</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Création des interfaces graphiques</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Implémentation de la base de données</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Implémentation de la base de données</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Implémentation de la base de données</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Absence - Imprévus</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Absence - Imprévus</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Relation base de données - application</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Relation base de données - application</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Relation base de données - application</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Relation base de données - application</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Relation base de données - application</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Absence - Imprévus</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Fonctionnalités du programme</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Fonctionnalités du programme</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Autres points techniques</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Autres points techniques</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Absence - Imprévus</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Gestion des données utilisateur</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>Absence - Imprévus</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Autres points techniques</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Autres points techniques</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>Documentation et modèles structurants</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>Documentation et modèles structurants</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>Documentation et modèles structurants</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Documentation et modèles structurants</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Documentation et modèles structurants</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Documentation et modèles structurants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphique-JNLTRAV'!$B$2:$B$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="67"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8A0F-4004-9507-727898CE9D77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="761183104"/>
+        <c:axId val="755994784"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="761183104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="755994784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="755994784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="761183104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2500,7 +3221,552 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3456,7 +4722,48 @@
         <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ABA34B8-1581-EA06-9EBB-E8B18417F662}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7D4BF5A-72A1-4FCB-2CFD-D71BE5880BA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3709,8 +5016,8 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView view="pageBreakPreview" topLeftCell="B5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4772,27 +6079,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -4822,27 +6129,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5315,7 +6622,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6148,8 +7455,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6203,7 +7510,7 @@
       <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="96" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="2">
@@ -6279,7 +7586,7 @@
         <v>56</v>
       </c>
       <c r="D9" s="94" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
@@ -6568,7 +7875,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="93" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="D32" s="94" t="s">
         <v>83</v>
@@ -6582,7 +7889,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" s="10"/>
     </row>
@@ -6611,7 +7918,7 @@
         <v>86</v>
       </c>
       <c r="D35" s="94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="27" x14ac:dyDescent="0.25">
@@ -6622,7 +7929,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D36" s="10"/>
     </row>
@@ -6634,7 +7941,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="10"/>
     </row>
@@ -6646,10 +7953,10 @@
         <v>4</v>
       </c>
       <c r="C38" s="93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
@@ -6660,10 +7967,10 @@
         <v>4</v>
       </c>
       <c r="C39" s="93" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="93" t="s">
         <v>93</v>
-      </c>
-      <c r="D39" s="93" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
@@ -6674,7 +7981,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="93" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D40" s="10"/>
     </row>
@@ -6686,7 +7993,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D41" s="10"/>
     </row>
@@ -6698,7 +8005,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D42" s="99"/>
     </row>
@@ -6710,10 +8017,10 @@
         <v>4</v>
       </c>
       <c r="C43" s="93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43" s="94" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="27" x14ac:dyDescent="0.25">
@@ -6724,7 +8031,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="93" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D44" s="10"/>
     </row>
@@ -6736,7 +8043,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D45" s="10"/>
     </row>
@@ -6748,7 +8055,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46" s="10"/>
     </row>
@@ -6760,7 +8067,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D47" s="10"/>
     </row>
@@ -6772,7 +8079,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="93" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D48" s="10"/>
     </row>
@@ -6784,10 +8091,10 @@
         <v>4</v>
       </c>
       <c r="C49" s="100" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D49" s="94" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
@@ -6798,10 +8105,10 @@
         <v>4</v>
       </c>
       <c r="C50" s="93" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" s="94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="81" x14ac:dyDescent="0.25">
@@ -6812,10 +8119,10 @@
         <v>4</v>
       </c>
       <c r="C51" s="93" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="93" t="s">
         <v>109</v>
-      </c>
-      <c r="D51" s="93" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="27" x14ac:dyDescent="0.25">
@@ -6826,7 +8133,7 @@
         <v>4</v>
       </c>
       <c r="C52" s="93" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="10"/>
     </row>
@@ -6838,7 +8145,7 @@
         <v>3</v>
       </c>
       <c r="C53" s="93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D53" s="10"/>
     </row>
@@ -6866,7 +8173,7 @@
     </row>
     <row r="57" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="107" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B57" s="108"/>
       <c r="C57" s="108"/>
@@ -6880,10 +8187,10 @@
         <v>4</v>
       </c>
       <c r="C58" s="93" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D58" s="93" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
@@ -6894,7 +8201,7 @@
         <v>4</v>
       </c>
       <c r="C59" s="93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D59" s="10"/>
     </row>
@@ -6906,10 +8213,10 @@
         <v>4</v>
       </c>
       <c r="C60" s="93" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D60" s="94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="54" x14ac:dyDescent="0.25">
@@ -6920,10 +8227,10 @@
         <v>4</v>
       </c>
       <c r="C61" s="93" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D61" s="94" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="27" x14ac:dyDescent="0.25">
@@ -6934,7 +8241,7 @@
         <v>4</v>
       </c>
       <c r="C62" s="93" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D62" s="10"/>
     </row>
@@ -6946,19 +8253,19 @@
         <v>4</v>
       </c>
       <c r="C63" s="101" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="10"/>
+    </row>
+    <row r="64" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A64" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="2">
+        <v>4</v>
+      </c>
+      <c r="C64" s="93" t="s">
         <v>121</v>
-      </c>
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A64" s="110" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" s="2">
-        <v>4</v>
-      </c>
-      <c r="C64" s="93" t="s">
-        <v>122</v>
       </c>
       <c r="D64" s="10"/>
     </row>
@@ -6970,7 +8277,7 @@
         <v>4</v>
       </c>
       <c r="C65" s="93" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D65" s="10"/>
     </row>
@@ -6982,7 +8289,7 @@
         <v>4</v>
       </c>
       <c r="C66" s="93" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D66" s="10"/>
     </row>
@@ -6994,7 +8301,7 @@
         <v>2</v>
       </c>
       <c r="C67" s="93" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D67" s="10"/>
     </row>
@@ -7006,7 +8313,7 @@
         <v>2</v>
       </c>
       <c r="C68" s="93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D68" s="10"/>
     </row>
@@ -7018,10 +8325,10 @@
         <v>4</v>
       </c>
       <c r="C69" s="93" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D69" s="102" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="27" x14ac:dyDescent="0.25">
@@ -7032,7 +8339,7 @@
         <v>4</v>
       </c>
       <c r="C70" s="93" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D70" s="10"/>
     </row>
@@ -7044,19 +8351,19 @@
         <v>4</v>
       </c>
       <c r="C71" s="93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A72" s="110" t="s">
+      <c r="A72" s="96" t="s">
         <v>33</v>
       </c>
       <c r="B72" s="2">
         <v>4</v>
       </c>
       <c r="C72" s="93" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D72" s="10"/>
     </row>
@@ -7068,7 +8375,7 @@
         <v>4</v>
       </c>
       <c r="C73" s="93" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D73" s="10"/>
     </row>
@@ -7080,7 +8387,7 @@
         <v>4</v>
       </c>
       <c r="C74" s="93" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D74" s="10"/>
     </row>
@@ -7092,20 +8399,32 @@
         <v>2</v>
       </c>
       <c r="C75" s="93" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="10"/>
+    <row r="76" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A76" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" s="2">
+        <v>4</v>
+      </c>
+      <c r="C76" s="93" t="s">
+        <v>140</v>
+      </c>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="10"/>
+    <row r="77" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A77" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" s="2">
+        <v>4</v>
+      </c>
+      <c r="C77" s="93" t="s">
+        <v>141</v>
+      </c>
       <c r="D77" s="10"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -7148,7 +8467,7 @@
       </c>
       <c r="B82" s="48">
         <f>SUM(B27:B81)</f>
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C82" s="90" t="s">
         <v>37</v>
@@ -7251,7 +8570,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7262,10 +8581,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
         <v>136</v>
-      </c>
-      <c r="B1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -7360,11 +8679,578 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14">
         <f>SUM(B2:B12)</f>
         <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B861D03F-F65D-4620-BF16-E46C8264B0DB}">
+  <dimension ref="A1:B68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:B21">JNLTRAV!A3:B22</f>
+        <v>Absence - Imprévus</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <v>Préparation au projet</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <v>Préparation au projet</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <v>Préparation au projet</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <v>Préparation au projet</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <v>Création des interfaces graphiques</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <v>Création des interfaces graphiques</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <v>Création des interfaces graphiques</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <v>Implémentation de la base de données</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <v>Implémentation de la base de données</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <v>Implémentation de la base de données</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <v>Absence - Imprévus</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <v>Absence - Imprévus</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <v>Relation base de données - application</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <v>Relation base de données - application</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <v>Relation base de données - application</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <v>Relation base de données - application</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <v>Relation base de données - application</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <v>Absence - Imprévus</v>
+      </c>
+      <c r="B21">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="str" cm="1">
+        <f t="array" ref="A22:B49">JNLTRAV!A27:B54</f>
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <v>Fonctionnalités du programme</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <v>Fonctionnalités du programme</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <v>Autres points techniques</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <v>Autres points techniques</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <v>Absence - Imprévus</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="str" cm="1">
+        <f t="array" ref="A50:B68">JNLTRAV!A58:B76</f>
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="str">
+        <v>Gestion des données utilisateur</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="str">
+        <v>Absence - Imprévus</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <v>Autres points techniques</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
+        <v>Autres points techniques</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
+        <v>Documentation et modèles structurants</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
+        <v>Documentation et modèles structurants</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <v>Documentation et modèles structurants</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <v>Documentation et modèles structurants</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <v>Documentation et modèles structurants</v>
+      </c>
+      <c r="B67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
+        <v>Documentation et modèles structurants</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -7385,15 +9271,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -7614,6 +9491,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
@@ -7626,14 +9512,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7650,4 +9528,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : items of contextual menu cleared
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65508A48-2834-4313-A0C6-D11563AE78CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C396EFA7-1D52-4373-ABF2-5036B6540E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="148">
   <si>
     <t>Module :</t>
   </si>
@@ -1018,6 +1018,27 @@
   </si>
   <si>
     <t>Mise au propre.</t>
+  </si>
+  <si>
+    <t>Améliorations</t>
+  </si>
+  <si>
+    <t>Insertion d'une puce pour plus de lisiblité.
+Découverte du fonctionnement de listview.
+Recherche solutions pour fermer le menu contextuel (3 options testées)</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/43841962/how-to-add-list-items-to-a-listview-in-cwinform
+c# 4.0 - C# - How to disable context menu in window form? - Stack Overflow</t>
+  </si>
+  <si>
+    <t>c# - Adding and removing ToolStripMenuItem's from MenuStrip and DropDownItems in WinForms - Stack Overflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solution transitoire trouvée pour la fermeture du menu contextuel : effacer les éléments du menu contextuel. </t>
+  </si>
+  <si>
+    <t>Recherche solution définitive.</t>
   </si>
 </sst>
 </file>
@@ -4763,7 +4784,7 @@
         <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7D4BF5A-72A1-4FCB-2CFD-D71BE5880BA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6622,7 +6643,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7453,10 +7474,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7464,7 +7485,7 @@
     <col min="1" max="1" width="21.42578125" style="29" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="29" customWidth="1"/>
     <col min="3" max="3" width="87" style="29" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="65" style="29" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="29"/>
   </cols>
   <sheetData>
@@ -8269,7 +8290,7 @@
       </c>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A65" s="96" t="s">
         <v>31</v>
       </c>
@@ -8281,7 +8302,7 @@
       </c>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A66" s="96" t="s">
         <v>31</v>
       </c>
@@ -8293,7 +8314,7 @@
       </c>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A67" s="96" t="s">
         <v>31</v>
       </c>
@@ -8305,7 +8326,7 @@
       </c>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="96" t="s">
         <v>21</v>
       </c>
@@ -8317,7 +8338,7 @@
       </c>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>35</v>
       </c>
@@ -8331,7 +8352,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>35</v>
       </c>
@@ -8343,7 +8364,7 @@
       </c>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>33</v>
       </c>
@@ -8355,7 +8376,7 @@
       </c>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A72" s="96" t="s">
         <v>33</v>
       </c>
@@ -8367,7 +8388,7 @@
       </c>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A73" s="96" t="s">
         <v>33</v>
       </c>
@@ -8379,7 +8400,7 @@
       </c>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A74" s="96" t="s">
         <v>33</v>
       </c>
@@ -8391,7 +8412,7 @@
       </c>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A75" s="96" t="s">
         <v>33</v>
       </c>
@@ -8403,7 +8424,7 @@
       </c>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A76" s="96" t="s">
         <v>33</v>
       </c>
@@ -8415,7 +8436,7 @@
       </c>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A77" s="96" t="s">
         <v>33</v>
       </c>
@@ -8427,92 +8448,179 @@
       </c>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="96"/>
       <c r="B78" s="2"/>
       <c r="C78" s="93"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="10"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="96"/>
+      <c r="C79" s="93"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="10"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="20"/>
-      <c r="H80" s="20"/>
-      <c r="I80" s="20"/>
-    </row>
-    <row r="81" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="10"/>
+    <row r="80" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B80" s="2">
+        <v>4</v>
+      </c>
+      <c r="C80" s="93" t="s">
+        <v>143</v>
+      </c>
+      <c r="D80" s="97" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B81" s="2">
+        <v>4</v>
+      </c>
+      <c r="C81" s="93" t="s">
+        <v>88</v>
+      </c>
       <c r="D81" s="10"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="33"/>
-      <c r="H81" s="34"/>
-      <c r="I81" s="20"/>
-    </row>
-    <row r="82" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="48" t="s">
+    </row>
+    <row r="82" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="A82" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" s="2">
+        <v>4</v>
+      </c>
+      <c r="C82" s="93" t="s">
+        <v>146</v>
+      </c>
+      <c r="D82" s="102" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2</v>
+      </c>
+      <c r="C83" s="93" t="s">
+        <v>147</v>
+      </c>
+      <c r="D83" s="10"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="96"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="93"/>
+      <c r="D84" s="10"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="96"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="93"/>
+      <c r="D85" s="10"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="96"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="93"/>
+      <c r="D86" s="10"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="96"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="93"/>
+      <c r="D87" s="10"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="93"/>
+      <c r="D88" s="10"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="20"/>
+      <c r="I90" s="20"/>
+    </row>
+    <row r="91" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="32"/>
+      <c r="G91" s="33"/>
+      <c r="H91" s="34"/>
+      <c r="I91" s="20"/>
+    </row>
+    <row r="92" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B82" s="48">
-        <f>SUM(B27:B81)</f>
-        <v>185</v>
-      </c>
-      <c r="C82" s="90" t="s">
+      <c r="B92" s="48">
+        <f>SUM(B27:B91)</f>
+        <v>199</v>
+      </c>
+      <c r="C92" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D82" s="49"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="20"/>
-      <c r="I82" s="20"/>
-    </row>
-    <row r="83" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A83" s="50"/>
-      <c r="B83" s="50"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="20"/>
-      <c r="G83" s="20"/>
-      <c r="H83" s="20"/>
-      <c r="I83" s="20"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="91" t="s">
+      <c r="D92" s="49"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="20"/>
+      <c r="H92" s="20"/>
+      <c r="I92" s="20"/>
+    </row>
+    <row r="93" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A93" s="50"/>
+      <c r="B93" s="50"/>
+      <c r="C93" s="50"/>
+      <c r="D93" s="50"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="20"/>
+      <c r="I93" s="20"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="20"/>
-      <c r="H84" s="20"/>
-      <c r="I84" s="20"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
+      <c r="H94" s="20"/>
+      <c r="I94" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B81" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B91" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B82" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B92" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A81" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A91" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -8530,16 +8638,18 @@
     <hyperlink ref="D61" r:id="rId11" xr:uid="{D9DF375C-7B06-4F91-B7AB-C5090DB2E41D}"/>
     <hyperlink ref="D69" r:id="rId12" display="https://riptutorial.com/csharp/example/20103/password-hashing" xr:uid="{08AF6903-8615-445A-9B9E-07607C69C38F}"/>
     <hyperlink ref="D9" r:id="rId13" display="https://www.youtube.com/watch?v=qFyRtrv-QDY" xr:uid="{91D49F7A-DAFE-41D3-851F-FF0E4C6B445F}"/>
+    <hyperlink ref="D80" r:id="rId14" location=" 4.0 - C# - How to disable context menu in window form? - Stack Overflow" xr:uid="{F809326F-5A8E-4C55-981C-692A5FE9666C}"/>
+    <hyperlink ref="D82" r:id="rId15" display="https://stackoverflow.com/questions/4041815/adding-and-removing-toolstripmenuitems-from-menustrip-and-dropdownitems-in-winf" xr:uid="{DF2A0308-5E77-4EF7-B9B1-AD308710AA8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
-  <drawing r:id="rId15"/>
-  <legacyDrawing r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <drawing r:id="rId17"/>
+  <legacyDrawing r:id="rId18"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId17" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+        <control shapeId="43009" r:id="rId19" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -8558,7 +8668,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId17" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId19" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -8569,7 +8679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3226A54-7399-49BB-B371-B772FF320D3A}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat : hash of data in database, management of global password hashed
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C396EFA7-1D52-4373-ABF2-5036B6540E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1641EC-11EC-4734-A9F3-69D9D08459B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="154">
   <si>
     <t>Module :</t>
   </si>
@@ -1038,7 +1038,44 @@
     <t xml:space="preserve">Solution transitoire trouvée pour la fermeture du menu contextuel : effacer les éléments du menu contextuel. </t>
   </si>
   <si>
-    <t>Recherche solution définitive.</t>
+    <t>Recherche solution définitive.
+Recherche solution pour avoir des paramètres optionnels dans une classe.</t>
+  </si>
+  <si>
+    <t>Définitions des tâches supplémentaires.
+Reprise du hachage du mot de passe.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nouvelle source suite à l'indisponibilité du premier lien :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://medium.com/@imAkash25/hashing-and-salting-passwords-in-c-0ee223f07e20</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.geeksforgeeks.org/c-sharp-randomly-generating-strings/</t>
+  </si>
+  <si>
+    <t>Code pour hacher le mot de passe lors de la vérification des infos de connexion et de la création de compte.
+Génération aléatoire du grain de sel.</t>
+  </si>
+  <si>
+    <t>Lien paramètre optionnel :
+Lien 2 types de variable :</t>
+  </si>
+  <si>
+    <t>Gestion mise . 
+Retour première remise avec chef de projet.</t>
   </si>
 </sst>
 </file>
@@ -1778,7 +1815,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2091,6 +2128,23 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -6100,27 +6154,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6150,27 +6204,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7474,10 +7528,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7610,7 +7664,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="53" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -7624,7 +7678,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="53" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="53" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -7702,7 +7756,7 @@
       </c>
       <c r="D16" s="94"/>
     </row>
-    <row r="17" spans="1:4" s="53" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" s="53" customFormat="1" ht="54" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -7716,7 +7770,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="53" customFormat="1" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="53" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -7742,7 +7796,7 @@
       </c>
       <c r="D19" s="94"/>
     </row>
-    <row r="20" spans="1:4" s="53" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -7914,7 +7968,7 @@
       </c>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A34" s="96" t="s">
         <v>31</v>
       </c>
@@ -7928,7 +7982,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A35" s="96" t="s">
         <v>31</v>
       </c>
@@ -7980,7 +8034,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="81" x14ac:dyDescent="0.25">
       <c r="A39" s="96" t="s">
         <v>31</v>
       </c>
@@ -8030,7 +8084,7 @@
       </c>
       <c r="D42" s="99"/>
     </row>
-    <row r="43" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A43" s="96" t="s">
         <v>31</v>
       </c>
@@ -8132,7 +8186,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A51" s="96" t="s">
         <v>32</v>
       </c>
@@ -8200,7 +8254,7 @@
       <c r="C57" s="108"/>
       <c r="D57" s="109"/>
     </row>
-    <row r="58" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A58" s="96" t="s">
         <v>31</v>
       </c>
@@ -8455,9 +8509,12 @@
       <c r="D78" s="10"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="96"/>
-      <c r="C79" s="93"/>
-      <c r="D79" s="10"/>
+      <c r="A79" s="110">
+        <v>45754</v>
+      </c>
+      <c r="B79" s="111"/>
+      <c r="C79" s="112"/>
+      <c r="D79" s="113"/>
     </row>
     <row r="80" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A80" s="96" t="s">
@@ -8473,7 +8530,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="96" t="s">
         <v>142</v>
       </c>
@@ -8485,7 +8542,7 @@
       </c>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A82" s="96" t="s">
         <v>142</v>
       </c>
@@ -8499,128 +8556,224 @@
         <v>145</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="27" x14ac:dyDescent="0.25">
       <c r="A83" s="96" t="s">
         <v>142</v>
       </c>
       <c r="B83" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C83" s="93" t="s">
         <v>147</v>
       </c>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="96"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="93"/>
-      <c r="D84" s="10"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="96"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="93"/>
+    <row r="84" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A84" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B84" s="2">
+        <v>4</v>
+      </c>
+      <c r="C84" s="93" t="s">
+        <v>153</v>
+      </c>
+      <c r="D84" s="93" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" s="2">
+        <v>4</v>
+      </c>
+      <c r="C85" s="93" t="s">
+        <v>88</v>
+      </c>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="96"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="93"/>
-      <c r="D86" s="10"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="96"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="93"/>
-      <c r="D87" s="10"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="93"/>
-      <c r="D88" s="10"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="10"/>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="110">
+        <v>45755</v>
+      </c>
+      <c r="B86" s="114"/>
+      <c r="C86" s="112"/>
+      <c r="D86" s="113"/>
+    </row>
+    <row r="87" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" s="2">
+        <v>4</v>
+      </c>
+      <c r="C87" s="93" t="s">
+        <v>148</v>
+      </c>
+      <c r="D87" s="93" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B88" s="2">
+        <v>4</v>
+      </c>
+      <c r="C88" s="93" t="s">
+        <v>151</v>
+      </c>
+      <c r="D88" s="94" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B89" s="2">
+        <v>4</v>
+      </c>
+      <c r="C89" s="93"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="96"/>
       <c r="B90" s="2"/>
-      <c r="C90" s="10"/>
+      <c r="C90" s="93"/>
       <c r="D90" s="10"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
-      <c r="G90" s="20"/>
-      <c r="H90" s="20"/>
-      <c r="I90" s="20"/>
-    </row>
-    <row r="91" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="96"/>
       <c r="B91" s="2"/>
-      <c r="C91" s="10"/>
+      <c r="C91" s="93"/>
       <c r="D91" s="10"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="32"/>
-      <c r="G91" s="33"/>
-      <c r="H91" s="34"/>
-      <c r="I91" s="20"/>
-    </row>
-    <row r="92" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="48" t="s">
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="96"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="93"/>
+      <c r="D92" s="10"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="96"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="93"/>
+      <c r="D93" s="10"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="96"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="93"/>
+      <c r="D94" s="10"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="96"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="93"/>
+      <c r="D95" s="10"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="96"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="93"/>
+      <c r="D96" s="10"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="96"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="93"/>
+      <c r="D97" s="10"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="93"/>
+      <c r="D98" s="10"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="20"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="20"/>
+      <c r="H100" s="20"/>
+      <c r="I100" s="20"/>
+    </row>
+    <row r="101" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="20"/>
+      <c r="F101" s="32"/>
+      <c r="G101" s="33"/>
+      <c r="H101" s="34"/>
+      <c r="I101" s="20"/>
+    </row>
+    <row r="102" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B92" s="48">
-        <f>SUM(B27:B91)</f>
-        <v>199</v>
-      </c>
-      <c r="C92" s="90" t="s">
+      <c r="B102" s="48">
+        <f>SUM(B27:B101)</f>
+        <v>221</v>
+      </c>
+      <c r="C102" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D92" s="49"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="20"/>
-      <c r="G92" s="20"/>
-      <c r="H92" s="20"/>
-      <c r="I92" s="20"/>
-    </row>
-    <row r="93" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A93" s="50"/>
-      <c r="B93" s="50"/>
-      <c r="C93" s="50"/>
-      <c r="D93" s="50"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="20"/>
-      <c r="G93" s="20"/>
-      <c r="H93" s="20"/>
-      <c r="I93" s="20"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="91" t="s">
+      <c r="D102" s="49"/>
+      <c r="E102" s="20"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="20"/>
+      <c r="H102" s="20"/>
+      <c r="I102" s="20"/>
+    </row>
+    <row r="103" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A103" s="50"/>
+      <c r="B103" s="50"/>
+      <c r="C103" s="50"/>
+      <c r="D103" s="50"/>
+      <c r="E103" s="20"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="20"/>
+      <c r="H103" s="20"/>
+      <c r="I103" s="20"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="20"/>
-      <c r="H94" s="20"/>
-      <c r="I94" s="20"/>
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="20"/>
+      <c r="H104" s="20"/>
+      <c r="I104" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B91" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B101" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B92" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B102" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A91" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A101" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -8640,16 +8793,17 @@
     <hyperlink ref="D9" r:id="rId13" display="https://www.youtube.com/watch?v=qFyRtrv-QDY" xr:uid="{91D49F7A-DAFE-41D3-851F-FF0E4C6B445F}"/>
     <hyperlink ref="D80" r:id="rId14" location=" 4.0 - C# - How to disable context menu in window form? - Stack Overflow" xr:uid="{F809326F-5A8E-4C55-981C-692A5FE9666C}"/>
     <hyperlink ref="D82" r:id="rId15" display="https://stackoverflow.com/questions/4041815/adding-and-removing-toolstripmenuitems-from-menustrip-and-dropdownitems-in-winf" xr:uid="{DF2A0308-5E77-4EF7-B9B1-AD308710AA8F}"/>
+    <hyperlink ref="D88" r:id="rId16" xr:uid="{66BB8505-85A5-464B-A54A-7B5DD9E3EA68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
-  <drawing r:id="rId17"/>
-  <legacyDrawing r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <drawing r:id="rId18"/>
+  <legacyDrawing r:id="rId19"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId19" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+        <control shapeId="43009" r:id="rId20" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -8668,7 +8822,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId19" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId20" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -9381,6 +9535,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -9601,15 +9764,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
@@ -9622,6 +9776,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9638,12 +9800,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix : display of tasksTodo with the ones created im AddTaskPage.cs during the same login
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1641EC-11EC-4734-A9F3-69D9D08459B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F3BE2E-2844-4A9C-A699-8148652F3B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="158">
   <si>
     <t>Module :</t>
   </si>
@@ -1070,12 +1070,60 @@
 Génération aléatoire du grain de sel.</t>
   </si>
   <si>
-    <t>Lien paramètre optionnel :
+    <r>
+      <t>Lien paramètre optionnel :</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://learn.microsoft.com/fr-fr/dotnet/csharp/programming-guide/classes-and-structs/named-and-optional-arguments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 Lien 2 types de variable :</t>
-  </si>
-  <si>
-    <t>Gestion mise . 
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://www.webdevtutor.net/blog/c-sharp-variable-with-multiple-types</t>
+    </r>
+  </si>
+  <si>
+    <t>Gestion effacage textbox et label en une classe (voir la classe "EmptyUserInsert "). 
 Retour première remise avec chef de projet.</t>
+  </si>
+  <si>
+    <t>Problème lors de l'utilisation de la vérifiaction de l'authentification.
+Recherche solutions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hachage mis de côté.
+</t>
+  </si>
+  <si>
+    <t>Problème création de compte.</t>
+  </si>
+  <si>
+    <t>///
+Affichage des tâches à faire mis à jour en incluant les tâches ajoutées durant une même session.</t>
   </si>
 </sst>
 </file>
@@ -2109,6 +2157,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2128,23 +2193,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -5309,10 +5357,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="103" t="s">
+      <c r="B19" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="104"/>
+      <c r="C19" s="109"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -6263,7 +6311,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="110" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -6272,7 +6320,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="106"/>
+      <c r="B4" s="111"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -7530,8 +7578,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8247,12 +8295,12 @@
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="107" t="s">
+      <c r="A57" s="112" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="108"/>
-      <c r="C57" s="108"/>
-      <c r="D57" s="109"/>
+      <c r="B57" s="113"/>
+      <c r="C57" s="113"/>
+      <c r="D57" s="114"/>
     </row>
     <row r="58" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A58" s="96" t="s">
@@ -8509,12 +8557,12 @@
       <c r="D78" s="10"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="110">
+      <c r="A79" s="107">
         <v>45754</v>
       </c>
-      <c r="B79" s="111"/>
-      <c r="C79" s="112"/>
-      <c r="D79" s="113"/>
+      <c r="B79" s="103"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="105"/>
     </row>
     <row r="80" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A80" s="96" t="s">
@@ -8568,7 +8616,7 @@
       </c>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A84" s="96" t="s">
         <v>21</v>
       </c>
@@ -8595,12 +8643,12 @@
       <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="110">
+      <c r="A86" s="107">
         <v>45755</v>
       </c>
-      <c r="B86" s="114"/>
-      <c r="C86" s="112"/>
-      <c r="D86" s="113"/>
+      <c r="B86" s="106"/>
+      <c r="C86" s="104"/>
+      <c r="D86" s="105"/>
     </row>
     <row r="87" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A87" s="96" t="s">
@@ -8637,37 +8685,69 @@
       <c r="B89" s="2">
         <v>4</v>
       </c>
-      <c r="C89" s="93"/>
+      <c r="C89" s="93" t="s">
+        <v>88</v>
+      </c>
       <c r="D89" s="10"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="96"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="93"/>
+      <c r="A90" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B90" s="2">
+        <v>4</v>
+      </c>
+      <c r="C90" s="93" t="s">
+        <v>88</v>
+      </c>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="96"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="93"/>
+    <row r="91" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A91" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B91" s="2">
+        <v>4</v>
+      </c>
+      <c r="C91" s="93" t="s">
+        <v>154</v>
+      </c>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="96"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="93"/>
+    <row r="92" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A92" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B92" s="2">
+        <v>4</v>
+      </c>
+      <c r="C92" s="93" t="s">
+        <v>155</v>
+      </c>
       <c r="D92" s="10"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="96"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="93"/>
+      <c r="A93" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B93" s="2">
+        <v>4</v>
+      </c>
+      <c r="C93" s="93" t="s">
+        <v>156</v>
+      </c>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="96"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="93"/>
+    <row r="94" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B94" s="2">
+        <v>4</v>
+      </c>
+      <c r="C94" s="93" t="s">
+        <v>157</v>
+      </c>
       <c r="D94" s="10"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -8728,7 +8808,7 @@
       </c>
       <c r="B102" s="48">
         <f>SUM(B27:B101)</f>
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C102" s="90" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
style: MCD model restyled
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F3BE2E-2844-4A9C-A699-8148652F3B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDA27F9-D1E4-4BF1-94AB-D57059D9CFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="159">
   <si>
     <t>Module :</t>
   </si>
@@ -1124,6 +1124,9 @@
   <si>
     <t>///
 Affichage des tâches à faire mis à jour en incluant les tâches ajoutées durant une même session.</t>
+  </si>
+  <si>
+    <t>Mise en place du modèle MVC revisé.</t>
   </si>
 </sst>
 </file>
@@ -1863,7 +1866,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2196,6 +2199,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -6202,27 +6214,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6252,27 +6264,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7576,10 +7588,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8750,110 +8762,178 @@
       </c>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="96"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="93"/>
-      <c r="D95" s="10"/>
+    <row r="95" spans="1:4" s="117" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A95" s="107">
+        <v>45756</v>
+      </c>
+      <c r="B95" s="115"/>
+      <c r="C95" s="116"/>
+      <c r="D95" s="116"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="96"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="93"/>
+      <c r="A96" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B96" s="2">
+        <v>4</v>
+      </c>
+      <c r="C96" s="93" t="s">
+        <v>158</v>
+      </c>
       <c r="D96" s="10"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="96"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="93"/>
+      <c r="A97" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B97" s="2">
+        <v>4</v>
+      </c>
+      <c r="C97" s="93" t="s">
+        <v>88</v>
+      </c>
       <c r="D97" s="10"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="93"/>
+      <c r="A98" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B98" s="2">
+        <v>2</v>
+      </c>
+      <c r="C98" s="93" t="s">
+        <v>88</v>
+      </c>
       <c r="D98" s="10"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
+      <c r="A99" s="96"/>
       <c r="B99" s="2"/>
-      <c r="C99" s="10"/>
+      <c r="C99" s="93"/>
       <c r="D99" s="10"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
+      <c r="A100" s="96"/>
       <c r="B100" s="2"/>
-      <c r="C100" s="10"/>
+      <c r="C100" s="93"/>
       <c r="D100" s="10"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="20"/>
-      <c r="G100" s="20"/>
-      <c r="H100" s="20"/>
-      <c r="I100" s="20"/>
-    </row>
-    <row r="101" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="96"/>
       <c r="B101" s="2"/>
-      <c r="C101" s="10"/>
+      <c r="C101" s="93"/>
       <c r="D101" s="10"/>
-      <c r="E101" s="20"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="33"/>
-      <c r="H101" s="34"/>
-      <c r="I101" s="20"/>
-    </row>
-    <row r="102" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="48" t="s">
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="96"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="93"/>
+      <c r="D102" s="10"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="96"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="93"/>
+      <c r="D103" s="10"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="96"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="93"/>
+      <c r="D104" s="10"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="96"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="93"/>
+      <c r="D105" s="10"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="93"/>
+      <c r="D106" s="10"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="20"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="20"/>
+      <c r="I108" s="20"/>
+    </row>
+    <row r="109" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="20"/>
+      <c r="F109" s="32"/>
+      <c r="G109" s="33"/>
+      <c r="H109" s="34"/>
+      <c r="I109" s="20"/>
+    </row>
+    <row r="110" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B102" s="48">
-        <f>SUM(B27:B101)</f>
-        <v>241</v>
-      </c>
-      <c r="C102" s="90" t="s">
+      <c r="B110" s="48">
+        <f>SUM(B27:B109)</f>
+        <v>251</v>
+      </c>
+      <c r="C110" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D102" s="49"/>
-      <c r="E102" s="20"/>
-      <c r="F102" s="20"/>
-      <c r="G102" s="20"/>
-      <c r="H102" s="20"/>
-      <c r="I102" s="20"/>
-    </row>
-    <row r="103" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A103" s="50"/>
-      <c r="B103" s="50"/>
-      <c r="C103" s="50"/>
-      <c r="D103" s="50"/>
-      <c r="E103" s="20"/>
-      <c r="F103" s="20"/>
-      <c r="G103" s="20"/>
-      <c r="H103" s="20"/>
-      <c r="I103" s="20"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="91" t="s">
+      <c r="D110" s="49"/>
+      <c r="E110" s="20"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="20"/>
+      <c r="H110" s="20"/>
+      <c r="I110" s="20"/>
+    </row>
+    <row r="111" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A111" s="50"/>
+      <c r="B111" s="50"/>
+      <c r="C111" s="50"/>
+      <c r="D111" s="50"/>
+      <c r="E111" s="20"/>
+      <c r="F111" s="20"/>
+      <c r="G111" s="20"/>
+      <c r="H111" s="20"/>
+      <c r="I111" s="20"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="20"/>
-      <c r="H104" s="20"/>
-      <c r="I104" s="20"/>
+      <c r="E112" s="20"/>
+      <c r="F112" s="20"/>
+      <c r="G112" s="20"/>
+      <c r="H112" s="20"/>
+      <c r="I112" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B101" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B109" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B102" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B110" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A101" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A109" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -9615,15 +9695,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -9844,6 +9915,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
@@ -9856,14 +9936,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9880,4 +9952,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
style : MVC model restyled next
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDA27F9-D1E4-4BF1-94AB-D57059D9CFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B41B60C-40D3-4A95-8C66-D237A7CEB305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11760" yWindow="5880" windowWidth="14445" windowHeight="11385" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="162">
   <si>
     <t>Module :</t>
   </si>
@@ -1127,6 +1127,16 @@
   </si>
   <si>
     <t>Mise en place du modèle MVC revisé.</t>
+  </si>
+  <si>
+    <t>Mise en place du modèle MVC revisé (gestion des events).</t>
+  </si>
+  <si>
+    <t>Classe "RemoveTask" supprimée pour plus de simplification et de logique.
+Gestion de la fermeture du menu contextuel.</t>
+  </si>
+  <si>
+    <t>Affichage de la liste des tâches après qu'une tâche ait été marquée comme faite.</t>
   </si>
 </sst>
 </file>
@@ -2177,6 +2187,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2199,15 +2218,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -5369,10 +5379,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="109"/>
+      <c r="C19" s="112"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -6214,27 +6224,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6264,27 +6274,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -6323,7 +6333,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="113" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -6332,7 +6342,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="111"/>
+      <c r="B4" s="114"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -7588,10 +7598,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8307,12 +8317,12 @@
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="112" t="s">
+      <c r="A57" s="115" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="113"/>
-      <c r="C57" s="113"/>
-      <c r="D57" s="114"/>
+      <c r="B57" s="116"/>
+      <c r="C57" s="116"/>
+      <c r="D57" s="117"/>
     </row>
     <row r="58" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A58" s="96" t="s">
@@ -8762,13 +8772,13 @@
       </c>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="1:4" s="117" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" s="110" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="107">
         <v>45756</v>
       </c>
-      <c r="B95" s="115"/>
-      <c r="C95" s="116"/>
-      <c r="D95" s="116"/>
+      <c r="B95" s="108"/>
+      <c r="C95" s="109"/>
+      <c r="D95" s="109"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="96" t="s">
@@ -8782,7 +8792,7 @@
       </c>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="96" t="s">
         <v>142</v>
       </c>
@@ -8794,7 +8804,7 @@
       </c>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="96" t="s">
         <v>142</v>
       </c>
@@ -8806,134 +8816,226 @@
       </c>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="96"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="93"/>
-      <c r="D99" s="10"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="96"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="93"/>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="107">
+        <v>45757</v>
+      </c>
+      <c r="B99" s="108"/>
+      <c r="C99" s="109"/>
+      <c r="D99" s="109"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B100" s="2">
+        <v>4</v>
+      </c>
+      <c r="C100" s="93" t="s">
+        <v>159</v>
+      </c>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="96"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="93"/>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B101" s="2">
+        <v>4</v>
+      </c>
+      <c r="C101" s="93" t="s">
+        <v>88</v>
+      </c>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="96"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="93"/>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B102" s="2">
+        <v>4</v>
+      </c>
+      <c r="C102" s="93" t="s">
+        <v>88</v>
+      </c>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="96"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="93"/>
+    <row r="103" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A103" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B103" s="2">
+        <v>4</v>
+      </c>
+      <c r="C103" s="93" t="s">
+        <v>160</v>
+      </c>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="96"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="93"/>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B104" s="2">
+        <v>2</v>
+      </c>
+      <c r="C104" s="93" t="s">
+        <v>161</v>
+      </c>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="96"/>
       <c r="B105" s="2"/>
       <c r="C105" s="93"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="96"/>
       <c r="B106" s="2"/>
       <c r="C106" s="93"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="96"/>
       <c r="B107" s="2"/>
-      <c r="C107" s="10"/>
+      <c r="C107" s="93"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="96"/>
       <c r="B108" s="2"/>
-      <c r="C108" s="10"/>
+      <c r="C108" s="93"/>
       <c r="D108" s="10"/>
-      <c r="E108" s="20"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="20"/>
-      <c r="H108" s="20"/>
-      <c r="I108" s="20"/>
-    </row>
-    <row r="109" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="1"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="96"/>
       <c r="B109" s="2"/>
-      <c r="C109" s="10"/>
+      <c r="C109" s="93"/>
       <c r="D109" s="10"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="32"/>
-      <c r="G109" s="33"/>
-      <c r="H109" s="34"/>
-      <c r="I109" s="20"/>
-    </row>
-    <row r="110" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="48" t="s">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="96"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="93"/>
+      <c r="D110" s="10"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="96"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="93"/>
+      <c r="D111" s="10"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="96"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="93"/>
+      <c r="D112" s="10"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="96"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="93"/>
+      <c r="D113" s="10"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="96"/>
+      <c r="B114" s="2"/>
+      <c r="C114" s="93"/>
+      <c r="D114" s="10"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="96"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="93"/>
+      <c r="D115" s="10"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="93"/>
+      <c r="D116" s="10"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="10"/>
+      <c r="D118" s="10"/>
+      <c r="E118" s="20"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="20"/>
+      <c r="H118" s="20"/>
+      <c r="I118" s="20"/>
+    </row>
+    <row r="119" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="20"/>
+      <c r="F119" s="32"/>
+      <c r="G119" s="33"/>
+      <c r="H119" s="34"/>
+      <c r="I119" s="20"/>
+    </row>
+    <row r="120" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B110" s="48">
-        <f>SUM(B27:B109)</f>
-        <v>251</v>
-      </c>
-      <c r="C110" s="90" t="s">
+      <c r="B120" s="48">
+        <f>SUM(B27:B119)</f>
+        <v>269</v>
+      </c>
+      <c r="C120" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D110" s="49"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="20"/>
-      <c r="I110" s="20"/>
-    </row>
-    <row r="111" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A111" s="50"/>
-      <c r="B111" s="50"/>
-      <c r="C111" s="50"/>
-      <c r="D111" s="50"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="20"/>
-      <c r="H111" s="20"/>
-      <c r="I111" s="20"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="91" t="s">
+      <c r="D120" s="49"/>
+      <c r="E120" s="20"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="20"/>
+      <c r="H120" s="20"/>
+      <c r="I120" s="20"/>
+    </row>
+    <row r="121" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A121" s="50"/>
+      <c r="B121" s="50"/>
+      <c r="C121" s="50"/>
+      <c r="D121" s="50"/>
+      <c r="E121" s="20"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="20"/>
+      <c r="H121" s="20"/>
+      <c r="I121" s="20"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="20"/>
-      <c r="H112" s="20"/>
-      <c r="I112" s="20"/>
+      <c r="E122" s="20"/>
+      <c r="F122" s="20"/>
+      <c r="G122" s="20"/>
+      <c r="H122" s="20"/>
+      <c r="I122" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B109" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B119" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B110" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B120" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A109" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A119" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>
@@ -9695,6 +9797,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -9915,15 +10026,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
@@ -9936,6 +10038,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9952,12 +10062,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
style : TasksDonePage.cs display following the MVC model, fix : display of context menu once the page has been changed okay
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B41B60C-40D3-4A95-8C66-D237A7CEB305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0576310B-3F58-4615-B771-C4B1E403861A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="5880" windowWidth="14445" windowHeight="11385" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11760" yWindow="4215" windowWidth="14445" windowHeight="11385" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="164">
   <si>
     <t>Module :</t>
   </si>
@@ -1136,7 +1136,17 @@
 Gestion de la fermeture du menu contextuel.</t>
   </si>
   <si>
-    <t>Affichage de la liste des tâches après qu'une tâche ait été marquée comme faite.</t>
+    <t xml:space="preserve">Affichage de la liste des tâches après qu'une tâche ait été marquée comme faite.
+Problème au niveau de la fermeture du menu conceptuel.
+</t>
+  </si>
+  <si>
+    <t>Tâches de "TasksDonePage.cs"  affichées selon le modèle MVC.
+Reaffichage du menu conceptuel une fois qu'on a changé de page okay.
+Problème pour gérer les différentes tâches (tout se fait sur la dernière tâche affichée).</t>
+  </si>
+  <si>
+    <t>Utilisation du paramètre "sender" pour connaître le nom de la tâche cliquée et faire plus d'opérations.</t>
   </si>
 </sst>
 </file>
@@ -6224,27 +6234,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6274,27 +6284,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7600,8 +7610,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8872,28 +8882,40 @@
       </c>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A104" s="96" t="s">
         <v>142</v>
       </c>
       <c r="B104" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C104" s="93" t="s">
         <v>161</v>
       </c>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="96"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="93"/>
+    <row r="105" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B105" s="2">
+        <v>4</v>
+      </c>
+      <c r="C105" s="93" t="s">
+        <v>162</v>
+      </c>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="96"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="93"/>
+    <row r="106" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A106" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B106" s="2">
+        <v>4</v>
+      </c>
+      <c r="C106" s="93" t="s">
+        <v>163</v>
+      </c>
       <c r="D106" s="10"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -8990,7 +9012,7 @@
       </c>
       <c r="B120" s="48">
         <f>SUM(B27:B119)</f>
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="C120" s="90" t="s">
         <v>37</v>
@@ -9797,15 +9819,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -10026,6 +10039,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
@@ -10038,14 +10060,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10062,4 +10076,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix : recognition of the task clicked, acknowledge of the active task when changing form, close of contextual menu when task moved or erased
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0576310B-3F58-4615-B771-C4B1E403861A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981C1BC6-FC95-4BE9-8484-60027134DD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11760" yWindow="4215" windowWidth="14445" windowHeight="11385" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14130" yWindow="4215" windowWidth="14445" windowHeight="11385" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="170">
   <si>
     <t>Module :</t>
   </si>
@@ -1147,6 +1147,27 @@
   </si>
   <si>
     <t>Utilisation du paramètre "sender" pour connaître le nom de la tâche cliquée et faire plus d'opérations.</t>
+  </si>
+  <si>
+    <t>Tâche cliquée reconnue qu'importe son emplacement.
+Quand changement de page, difficulté à reconnaître la tâche active.</t>
+  </si>
+  <si>
+    <t>Tâche active reconnue quand changement de page.
+Fermeture du menu contextuel quand tâche déplacée ou effacée.</t>
+  </si>
+  <si>
+    <t>Recherche manière de gérer la fermeture du menu contextuel quand clic sur une autre tâche.
+Retour au label quand menu contextuel fermé après édition d'une tâche sans appui de la touche "enter".</t>
+  </si>
+  <si>
+    <t>Difficultés à "déplacer" une tâche vers un autre formualire et dans la base de données sans utilisation de l'éxécution pas à pas. - Autre débug donne un faux positif.</t>
+  </si>
+  <si>
+    <t>Recherche solution au problème lors du "déplacement" de la tâche.</t>
+  </si>
+  <si>
+    <t>ChatGPT.com</t>
   </si>
 </sst>
 </file>
@@ -7608,10 +7629,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292D540-B813-4507-A56B-AB5C19AE6197}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I122"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8919,145 +8940,275 @@
       <c r="D106" s="10"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="96"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="93"/>
-      <c r="D107" s="10"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="96"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="93"/>
+      <c r="A107" s="107">
+        <v>45758</v>
+      </c>
+      <c r="B107" s="106"/>
+      <c r="C107" s="104"/>
+      <c r="D107" s="105"/>
+    </row>
+    <row r="108" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A108" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B108" s="2">
+        <v>4</v>
+      </c>
+      <c r="C108" s="93" t="s">
+        <v>164</v>
+      </c>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="96"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="93"/>
+    <row r="109" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A109" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B109" s="2">
+        <v>4</v>
+      </c>
+      <c r="C109" s="93" t="s">
+        <v>165</v>
+      </c>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="96"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="93"/>
+    <row r="110" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="A110" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B110" s="2">
+        <v>4</v>
+      </c>
+      <c r="C110" s="93" t="s">
+        <v>166</v>
+      </c>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="96"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="93"/>
-      <c r="D111" s="10"/>
+    <row r="111" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A111" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B111" s="2">
+        <v>4</v>
+      </c>
+      <c r="C111" s="93" t="s">
+        <v>167</v>
+      </c>
+      <c r="D111" s="93" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="96"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="93"/>
+      <c r="A112" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B112" s="2">
+        <v>2</v>
+      </c>
+      <c r="C112" s="93" t="s">
+        <v>168</v>
+      </c>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="96"/>
       <c r="B113" s="2"/>
       <c r="C113" s="93"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="96"/>
       <c r="B114" s="2"/>
       <c r="C114" s="93"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="96"/>
       <c r="B115" s="2"/>
       <c r="C115" s="93"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="96"/>
       <c r="B116" s="2"/>
       <c r="C116" s="93"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="96"/>
       <c r="B117" s="2"/>
-      <c r="C117" s="10"/>
+      <c r="C117" s="93"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="96"/>
       <c r="B118" s="2"/>
-      <c r="C118" s="10"/>
+      <c r="C118" s="93"/>
       <c r="D118" s="10"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="20"/>
-      <c r="G118" s="20"/>
-      <c r="H118" s="20"/>
-      <c r="I118" s="20"/>
-    </row>
-    <row r="119" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="1"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="96"/>
       <c r="B119" s="2"/>
-      <c r="C119" s="10"/>
+      <c r="C119" s="93"/>
       <c r="D119" s="10"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="32"/>
-      <c r="G119" s="33"/>
-      <c r="H119" s="34"/>
-      <c r="I119" s="20"/>
-    </row>
-    <row r="120" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="48" t="s">
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="96"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="93"/>
+      <c r="D120" s="10"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="96"/>
+      <c r="B121" s="2"/>
+      <c r="C121" s="93"/>
+      <c r="D121" s="10"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="96"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="93"/>
+      <c r="D122" s="10"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="96"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="93"/>
+      <c r="D123" s="10"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="96"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="93"/>
+      <c r="D124" s="10"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="96"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="93"/>
+      <c r="D125" s="10"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="96"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="93"/>
+      <c r="D126" s="10"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="96"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="93"/>
+      <c r="D127" s="10"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="96"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="93"/>
+      <c r="D128" s="10"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="96"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="93"/>
+      <c r="D129" s="10"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="96"/>
+      <c r="B130" s="2"/>
+      <c r="C130" s="93"/>
+      <c r="D130" s="10"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="96"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="93"/>
+      <c r="D131" s="10"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="93"/>
+      <c r="D132" s="10"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="10"/>
+      <c r="D134" s="10"/>
+      <c r="E134" s="20"/>
+      <c r="F134" s="20"/>
+      <c r="G134" s="20"/>
+      <c r="H134" s="20"/>
+      <c r="I134" s="20"/>
+    </row>
+    <row r="135" spans="1:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="20"/>
+      <c r="F135" s="32"/>
+      <c r="G135" s="33"/>
+      <c r="H135" s="34"/>
+      <c r="I135" s="20"/>
+    </row>
+    <row r="136" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B120" s="48">
-        <f>SUM(B27:B119)</f>
-        <v>279</v>
-      </c>
-      <c r="C120" s="90" t="s">
+      <c r="B136" s="48">
+        <f>SUM(B27:B135)</f>
+        <v>297</v>
+      </c>
+      <c r="C136" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D120" s="49"/>
-      <c r="E120" s="20"/>
-      <c r="F120" s="20"/>
-      <c r="G120" s="20"/>
-      <c r="H120" s="20"/>
-      <c r="I120" s="20"/>
-    </row>
-    <row r="121" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A121" s="50"/>
-      <c r="B121" s="50"/>
-      <c r="C121" s="50"/>
-      <c r="D121" s="50"/>
-      <c r="E121" s="20"/>
-      <c r="F121" s="20"/>
-      <c r="G121" s="20"/>
-      <c r="H121" s="20"/>
-      <c r="I121" s="20"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="91" t="s">
+      <c r="D136" s="49"/>
+      <c r="E136" s="20"/>
+      <c r="F136" s="20"/>
+      <c r="G136" s="20"/>
+      <c r="H136" s="20"/>
+      <c r="I136" s="20"/>
+    </row>
+    <row r="137" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A137" s="50"/>
+      <c r="B137" s="50"/>
+      <c r="C137" s="50"/>
+      <c r="D137" s="50"/>
+      <c r="E137" s="20"/>
+      <c r="F137" s="20"/>
+      <c r="G137" s="20"/>
+      <c r="H137" s="20"/>
+      <c r="I137" s="20"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E122" s="20"/>
-      <c r="F122" s="20"/>
-      <c r="G122" s="20"/>
-      <c r="H122" s="20"/>
-      <c r="I122" s="20"/>
+      <c r="E138" s="20"/>
+      <c r="F138" s="20"/>
+      <c r="G138" s="20"/>
+      <c r="H138" s="20"/>
+      <c r="I138" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B119" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B135" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B120" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B136" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
       <formula1>0</formula1>
       <formula2>NbPerWeek * NbQuartPer</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A119" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A22 A27:A135" xr:uid="{FEF990B1-F98A-4F1C-9CC0-B3F738733A5B}">
       <formula1>lstTasks</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix : management of erreors on a task when in editing mode okay
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981C1BC6-FC95-4BE9-8484-60027134DD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC291AA-9FEB-4593-A350-56EE23C85229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14130" yWindow="4215" windowWidth="14445" windowHeight="11385" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="173">
   <si>
     <t>Module :</t>
   </si>
@@ -1164,10 +1164,21 @@
     <t>Difficultés à "déplacer" une tâche vers un autre formualire et dans la base de données sans utilisation de l'éxécution pas à pas. - Autre débug donne un faux positif.</t>
   </si>
   <si>
-    <t>Recherche solution au problème lors du "déplacement" de la tâche.</t>
-  </si>
-  <si>
     <t>ChatGPT.com</t>
+  </si>
+  <si>
+    <t>Changement de méthode pour déplacer une tâche : utilisation de la requête "Update" au lieu de "Insert" (proposition de ChatGpt) + optimisation des classses utilisées ("Mark..." et "Unmark..." du "Controller" supprimés).
+Problème : si tâche en mode modification, puis clic sur une autre tâche affichage du texte de la tâche précédente à l'emplacement de cette tâche cliquée.</t>
+  </si>
+  <si>
+    <t>Même problème.</t>
+  </si>
+  <si>
+    <t>Problème sur tâche en modification résolu.
+Gestion du déplacement d'une tâche vers un autre form quand modification en cours okay.</t>
+  </si>
+  <si>
+    <t>Retour à la gestion vérification du mot de passe (en cours).</t>
   </si>
 </sst>
 </file>
@@ -1907,7 +1918,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2247,6 +2258,10 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -6255,27 +6270,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6305,27 +6320,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7632,7 +7647,7 @@
   <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8994,37 +9009,55 @@
         <v>167</v>
       </c>
       <c r="D111" s="93" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A112" s="96" t="s">
         <v>142</v>
       </c>
       <c r="B112" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C112" s="93" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D112" s="10"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="96"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="93"/>
+      <c r="A113" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B113" s="2">
+        <v>4</v>
+      </c>
+      <c r="C113" s="93" t="s">
+        <v>170</v>
+      </c>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="96"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="93"/>
-      <c r="D114" s="10"/>
+    <row r="114" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B114" s="2">
+        <v>4</v>
+      </c>
+      <c r="C114" s="93" t="s">
+        <v>171</v>
+      </c>
+      <c r="D114" s="118"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="96"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="93"/>
+      <c r="A115" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B115" s="2">
+        <v>4</v>
+      </c>
+      <c r="C115" s="93" t="s">
+        <v>172</v>
+      </c>
       <c r="D115" s="10"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -9048,7 +9081,7 @@
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="96"/>
       <c r="B119" s="2"/>
-      <c r="C119" s="93"/>
+      <c r="C119" s="2"/>
       <c r="D119" s="10"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -9163,7 +9196,7 @@
       </c>
       <c r="B136" s="48">
         <f>SUM(B27:B135)</f>
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="C136" s="90" t="s">
         <v>37</v>
@@ -9201,7 +9234,7 @@
     <mergeCell ref="A57:D57"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B135" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
+    <dataValidation type="whole" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée en 1/3 de période" error="Le nombre doit être de type entier" sqref="B3:B22 B27:B56 B58:B78 B80:B135 C119" xr:uid="{A6A63D01-659D-4038-9B69-E9EE45524195}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="whole" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Dépassement de durée" error="Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B23 B136" xr:uid="{53D066D9-D4B4-4D3E-980E-A3E3E32CC2C7}">
@@ -9970,6 +10003,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -10190,15 +10232,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
@@ -10211,6 +10244,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10227,12 +10268,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat : triggers when update and delete, password hidden when writing, powerpoint done
</commit_message>
<xml_diff>
--- a/documents/Planification-jnltrav.xlsx
+++ b/documents/Planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sardongmo\Desktop\E_TodoList\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC291AA-9FEB-4593-A350-56EE23C85229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60987AED-3E74-4F3E-BB84-ACF475292B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="181">
   <si>
     <t>Module :</t>
   </si>
@@ -1179,6 +1179,34 @@
   </si>
   <si>
     <t>Retour à la gestion vérification du mot de passe (en cours).</t>
+  </si>
+  <si>
+    <t>Préparation présentation.
+Copie de la solution pour faire une version améliorée.</t>
+  </si>
+  <si>
+    <t>Mise en place d'une suppression données en cascade.
+Déclencheurs pour suppression et mise à jour des données.</t>
+  </si>
+  <si>
+    <t>Solution de simplification recommandée par ChatGPT.</t>
+  </si>
+  <si>
+    <t>Comment utiliser l’option CASCADE en SQL pour supprimer les enregistrements enfants avec le parent | IT trip</t>
+  </si>
+  <si>
+    <t>Simplification des triggers en utilisant "ON … CASCADE".
+Recherche manière de faire des tags sur "GitHub".</t>
+  </si>
+  <si>
+    <t>https://codebun.com/hide-and-show-password-text-using-checkbox-in-c-windows-application/</t>
+  </si>
+  <si>
+    <t>Mot de passe caché lors de la saisie.
+Modification modèles structurants (MCD et MLD).</t>
+  </si>
+  <si>
+    <t>Finalisation de la présentation.</t>
   </si>
 </sst>
 </file>
@@ -2238,6 +2266,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2258,10 +2290,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5425,10 +5453,10 @@
     </row>
     <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="111" t="s">
+      <c r="B19" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="112"/>
+      <c r="C19" s="113"/>
       <c r="D19" s="60"/>
       <c r="E19" s="60"/>
       <c r="F19" s="60"/>
@@ -6270,27 +6298,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -6320,27 +6348,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -6379,7 +6407,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="114" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -6388,7 +6416,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="114"/>
+      <c r="B4" s="115"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -7646,8 +7674,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8363,12 +8391,12 @@
       <c r="D56" s="10"/>
     </row>
     <row r="57" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="115" t="s">
+      <c r="A57" s="116" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="116"/>
-      <c r="C57" s="116"/>
-      <c r="D57" s="117"/>
+      <c r="B57" s="117"/>
+      <c r="C57" s="117"/>
+      <c r="D57" s="118"/>
     </row>
     <row r="58" spans="1:4" ht="54" x14ac:dyDescent="0.25">
       <c r="A58" s="96" t="s">
@@ -9046,7 +9074,7 @@
       <c r="C114" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="D114" s="118"/>
+      <c r="D114" s="111"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="96" t="s">
@@ -9079,39 +9107,77 @@
       <c r="D118" s="10"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="96"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="10"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="96"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="93"/>
+      <c r="A119" s="107">
+        <v>45775</v>
+      </c>
+      <c r="B119" s="108"/>
+      <c r="C119" s="108"/>
+      <c r="D119" s="109"/>
+    </row>
+    <row r="120" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A120" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B120" s="2">
+        <v>4</v>
+      </c>
+      <c r="C120" s="93" t="s">
+        <v>173</v>
+      </c>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="96"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="93"/>
-      <c r="D121" s="10"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="96"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="93"/>
-      <c r="D122" s="10"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="96"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="93"/>
-      <c r="D123" s="10"/>
+    <row r="121" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A121" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B121" s="2">
+        <v>4</v>
+      </c>
+      <c r="C121" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="D121" s="102" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A122" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B122" s="2">
+        <v>4</v>
+      </c>
+      <c r="C122" s="93" t="s">
+        <v>177</v>
+      </c>
+      <c r="D122" s="93" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A123" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B123" s="2">
+        <v>4</v>
+      </c>
+      <c r="C123" s="93" t="s">
+        <v>179</v>
+      </c>
+      <c r="D123" s="94" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="96"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="93"/>
+      <c r="A124" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="B124" s="2">
+        <v>4</v>
+      </c>
+      <c r="C124" s="93" t="s">
+        <v>180</v>
+      </c>
       <c r="D124" s="10"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -9196,7 +9262,7 @@
       </c>
       <c r="B136" s="48">
         <f>SUM(B27:B135)</f>
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="C136" s="90" t="s">
         <v>37</v>
@@ -9262,16 +9328,18 @@
     <hyperlink ref="D80" r:id="rId14" location=" 4.0 - C# - How to disable context menu in window form? - Stack Overflow" xr:uid="{F809326F-5A8E-4C55-981C-692A5FE9666C}"/>
     <hyperlink ref="D82" r:id="rId15" display="https://stackoverflow.com/questions/4041815/adding-and-removing-toolstripmenuitems-from-menustrip-and-dropdownitems-in-winf" xr:uid="{DF2A0308-5E77-4EF7-B9B1-AD308710AA8F}"/>
     <hyperlink ref="D88" r:id="rId16" xr:uid="{66BB8505-85A5-464B-A54A-7B5DD9E3EA68}"/>
+    <hyperlink ref="D121" r:id="rId17" display="https://fr.ittrip.xyz/sql/sql-cascade-delete" xr:uid="{0D731715-13AD-4F12-9DEF-DA1B2A9CF1BD}"/>
+    <hyperlink ref="D123" r:id="rId18" xr:uid="{C8CF4615-C37A-438A-9D4A-72D397E6850A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
-  <drawing r:id="rId18"/>
-  <legacyDrawing r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <drawing r:id="rId20"/>
+  <legacyDrawing r:id="rId21"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId20" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+        <control shapeId="43009" r:id="rId22" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -9290,7 +9358,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId20" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId22" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10003,15 +10071,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a2a625e4713a1206e22a4c67b5bce77a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="44987950040cbf76ec9c25f294fcc9dd" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -10232,6 +10291,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
@@ -10244,14 +10312,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B433C9A-8A3A-4D69-955C-F3F07BFE315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10268,4 +10328,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>